<commit_message>
refined the backlog, added security as a priority over build server
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -8,18 +8,19 @@
   </bookViews>
   <sheets>
     <sheet name="backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="types" sheetId="2" r:id="rId2"/>
+    <sheet name="drop-downs" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Statuses">types!$B$2:$B$6</definedName>
-    <definedName name="Types">types!$A$2</definedName>
+    <definedName name="Statuses">'drop-downs'!$B$2:$B$6</definedName>
+    <definedName name="Themes">'drop-downs'!$C$2:$C$4</definedName>
+    <definedName name="Types">'drop-downs'!$A$2</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -100,13 +101,94 @@
   </si>
   <si>
     <t>https://app.pluralsight.com/library/courses/teamcity-getting-started</t>
+  </si>
+  <si>
+    <t>Theme</t>
+  </si>
+  <si>
+    <t>Themes</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Technical Debt</t>
+  </si>
+  <si>
+    <t>Build Server</t>
+  </si>
+  <si>
+    <t>Claims - Big Picture</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/claims-based-identity-big-picture</t>
+  </si>
+  <si>
+    <t>Linux User and Group Management</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/lfcs-linux-user-group-management</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/group-policy-fundamentals</t>
+  </si>
+  <si>
+    <t>Windows Group Policy Fundemendals</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/active-directory-programming</t>
+  </si>
+  <si>
+    <t>Active Directory Programming</t>
+  </si>
+  <si>
+    <t>Oauth 2 Introduction</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/oauth2-json-web-tokens-openid-connect-introduction</t>
+  </si>
+  <si>
+    <t>Oauth ASP Api</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/oauth-secure-asp-dot-net-api</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/implementing-restful-aspdotnet-web-api</t>
+  </si>
+  <si>
+    <t>Securing ASP Api (chapter 3)</t>
+  </si>
+  <si>
+    <t>Oauth, ASP, Angular</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/oauth2-openid-connect-angular-aspdotnet</t>
+  </si>
+  <si>
+    <t>Securing multiple clients</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/building-securing-restful-api-aspdotnet</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>Read Oauth Specification</t>
+  </si>
+  <si>
+    <t>https://tools.ietf.org/html/rfc6749</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,13 +212,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2196ED"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -152,10 +247,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -163,6 +261,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF2196ED"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -461,246 +564,515 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="81.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="81.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="B2">
+      <c r="C12">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="B3">
+      <c r="C13">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="C14">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>18</v>
       </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>22</v>
       </c>
-      <c r="B6">
+      <c r="C16">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>21</v>
       </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>23</v>
       </c>
-      <c r="B8">
+      <c r="C18">
         <v>1</v>
       </c>
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>25</v>
       </c>
-      <c r="B9">
+      <c r="C19">
         <v>1</v>
       </c>
-      <c r="C9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C1048576 C2:C5">
+  <mergeCells count="1">
+    <mergeCell ref="A2:A7"/>
+  </mergeCells>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D15 D2:D4 D17:D19 D28:D1048576">
       <formula1>Types</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D1048576 D2:D5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E15 E2:E4 E17:E19 E28:E1048576">
       <formula1>Statuses</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4 F6:F19 F28:F1048576">
+      <formula1>Themes</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E4" r:id="rId2"/>
-    <hyperlink ref="E3" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="E7" r:id="rId5"/>
-    <hyperlink ref="E6" r:id="rId6"/>
-    <hyperlink ref="E8" r:id="rId7"/>
-    <hyperlink ref="E9" r:id="rId8"/>
+    <hyperlink ref="G12" r:id="rId1"/>
+    <hyperlink ref="G14" r:id="rId2"/>
+    <hyperlink ref="G13" r:id="rId3"/>
+    <hyperlink ref="G15" r:id="rId4"/>
+    <hyperlink ref="G17" r:id="rId5"/>
+    <hyperlink ref="G16" r:id="rId6"/>
+    <hyperlink ref="G18" r:id="rId7"/>
+    <hyperlink ref="G19" r:id="rId8"/>
+    <hyperlink ref="G2" r:id="rId9"/>
+    <hyperlink ref="G4" r:id="rId10"/>
+    <hyperlink ref="G3" r:id="rId11"/>
+    <hyperlink ref="G5" r:id="rId12"/>
+    <hyperlink ref="G6" r:id="rId13"/>
+    <hyperlink ref="G7" r:id="rId14"/>
+    <hyperlink ref="G8" r:id="rId15"/>
+    <hyperlink ref="G9" r:id="rId16"/>
+    <hyperlink ref="G10" r:id="rId17"/>
+    <hyperlink ref="G11" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating backlog for sprint 2
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -13,14 +13,14 @@
   <definedNames>
     <definedName name="Statuses">'drop-downs'!$B$2:$B$6</definedName>
     <definedName name="Themes">'drop-downs'!$C$2:$C$4</definedName>
-    <definedName name="Types">'drop-downs'!$A$2</definedName>
+    <definedName name="Types">'drop-downs'!$A$2:$A$3</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="90">
   <si>
     <t>Name</t>
   </si>
@@ -182,6 +182,114 @@
   </si>
   <si>
     <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Identity Server 4 + asp.core</t>
+  </si>
+  <si>
+    <t>Identity Server with Nhibernate stores</t>
+  </si>
+  <si>
+    <t>Angular 2 implicit/resource owner flow</t>
+  </si>
+  <si>
+    <t>Angular 2 token management</t>
+  </si>
+  <si>
+    <t>Refresh tokens</t>
+  </si>
+  <si>
+    <t>Login redirects</t>
+  </si>
+  <si>
+    <t>Logout redirects</t>
+  </si>
+  <si>
+    <t>Single sign-out</t>
+  </si>
+  <si>
+    <t>Impersonation</t>
+  </si>
+  <si>
+    <t>Google login</t>
+  </si>
+  <si>
+    <t>Microsoft login</t>
+  </si>
+  <si>
+    <t>WS-Federation + Windows login</t>
+  </si>
+  <si>
+    <t>Partial Logins</t>
+  </si>
+  <si>
+    <t>Client Management</t>
+  </si>
+  <si>
+    <t>Redirect tokens (implicit)</t>
+  </si>
+  <si>
+    <t>In order to create a proper POC, a simple identity server must be built in Identity Server 4 with asp.core; it must support access token, implicit, and resource owner flows</t>
+  </si>
+  <si>
+    <t>In order to create a proper POC, a simple identity server must be built which uses Fluent Nhibernate as a storage mechanism; it must support the resource owner flow.</t>
+  </si>
+  <si>
+    <t>In order to create a proper POC, 2 angular clients must be created, which can log in using either the implicit or resource owner flow.</t>
+  </si>
+  <si>
+    <t>In order to create a proper POC, an angular client must be created which can handle expired tokens for both implicit and resource owner flows.</t>
+  </si>
+  <si>
+    <t>In order to create a proper POC, clients must be created that can refresh their tokens; both resource owner and access token flows must be supported</t>
+  </si>
+  <si>
+    <t>In order to create a proper POC, a client must be created that can get a new token through redirection; when using the implicit flow.</t>
+  </si>
+  <si>
+    <t>In order to create a proper POC, clients must be created that can redirect to an application page after login; for resource owner, implicit, and access token flows.</t>
+  </si>
+  <si>
+    <t>In order to create a proper POC, clients must be created that can redirect the user to the applications login page; for resource owner, implicit, and access token flows.</t>
+  </si>
+  <si>
+    <t>In order to create a proper POC, clients must be created that force all other clients to log out; in resource owner, implitic, and access token flows.</t>
+  </si>
+  <si>
+    <t>In order to create a proper POC, resource servers must be able to filter and deny access to resources based on the user.</t>
+  </si>
+  <si>
+    <t>In order to create a proper POC, the identity server must be able to authenticate, link, and create users for a facebook account; must support resource owner, implicit, and access token flows.</t>
+  </si>
+  <si>
+    <t>In order to create a proper POC, the identity server must be able to authenticate, link, and create users for a Microsoft account; must support resource owner, implicit, and access token flows.</t>
+  </si>
+  <si>
+    <t>Facebook login</t>
+  </si>
+  <si>
+    <t>In order to create a proper POC, the identity server must be able to authenticate, link, and create users for a google account; must support resource owner, implicit, and access token flows.</t>
+  </si>
+  <si>
+    <t>In order to create a proper POC, the identity server must be able to authenticate, link, and create users for a Windows account; must support resource owner, implicit, and access token flows.</t>
+  </si>
+  <si>
+    <t>In order to create a proper POC, the identity server must be able to provide a page which allows users from an external provider to add missing claims; must support resource owner, implicit, and access token flows.</t>
+  </si>
+  <si>
+    <t>In order to create a proper POC, the identity server must provide an interface to manage applications which are authenticating against it.</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>SMWU Bugs</t>
+  </si>
+  <si>
+    <t>Fix the adding of blank rows.</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
   </si>
 </sst>
 </file>
@@ -220,7 +328,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,6 +338,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF2196ED"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF44336"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -247,11 +361,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -263,6 +380,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FFF44336"/>
       <color rgb="FF2196ED"/>
     </mruColors>
   </colors>
@@ -564,16 +682,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="81.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -601,7 +720,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>53</v>
       </c>
@@ -615,7 +734,7 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
         <v>29</v>
@@ -624,385 +743,744 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
         <v>29</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
         <v>29</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
         <v>29</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="G7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
       <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" t="s">
+        <v>31</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" t="s">
+        <v>31</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" t="s">
+        <v>29</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" t="s">
+        <v>29</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>45</v>
       </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="1" t="s">
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" t="s">
+        <v>29</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>48</v>
       </c>
-      <c r="C10">
+      <c r="C36">
         <v>3</v>
       </c>
-      <c r="D10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="D36" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" t="s">
+        <v>29</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" t="s">
-        <v>31</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" t="s">
-        <v>31</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" t="s">
-        <v>31</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" t="s">
-        <v>31</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" t="s">
-        <v>31</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:A7"/>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A23"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D15 D2:D4 D17:D19 D28:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2 D40:D1048576 D30:D36 D4:D28">
       <formula1>Types</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E15 E2:E4 E17:E19 E28:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E40:E1048576 E30:E36 E2:E28">
       <formula1>Statuses</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4 F6:F19 F28:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 F40:F1048576 F4:F36">
       <formula1>Themes</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G12" r:id="rId1"/>
-    <hyperlink ref="G14" r:id="rId2"/>
-    <hyperlink ref="G13" r:id="rId3"/>
-    <hyperlink ref="G15" r:id="rId4"/>
-    <hyperlink ref="G17" r:id="rId5"/>
-    <hyperlink ref="G16" r:id="rId6"/>
-    <hyperlink ref="G18" r:id="rId7"/>
-    <hyperlink ref="G19" r:id="rId8"/>
+    <hyperlink ref="G25" r:id="rId1"/>
+    <hyperlink ref="G27" r:id="rId2"/>
+    <hyperlink ref="G26" r:id="rId3"/>
+    <hyperlink ref="G28" r:id="rId4"/>
+    <hyperlink ref="G30" r:id="rId5"/>
+    <hyperlink ref="G29" r:id="rId6"/>
+    <hyperlink ref="G31" r:id="rId7"/>
+    <hyperlink ref="G32" r:id="rId8"/>
     <hyperlink ref="G2" r:id="rId9"/>
-    <hyperlink ref="G4" r:id="rId10"/>
-    <hyperlink ref="G3" r:id="rId11"/>
-    <hyperlink ref="G5" r:id="rId12"/>
-    <hyperlink ref="G6" r:id="rId13"/>
-    <hyperlink ref="G7" r:id="rId14"/>
-    <hyperlink ref="G8" r:id="rId15"/>
-    <hyperlink ref="G9" r:id="rId16"/>
-    <hyperlink ref="G10" r:id="rId17"/>
-    <hyperlink ref="G11" r:id="rId18"/>
+    <hyperlink ref="G34" r:id="rId10"/>
+    <hyperlink ref="G33" r:id="rId11"/>
+    <hyperlink ref="G3" r:id="rId12"/>
+    <hyperlink ref="G4" r:id="rId13"/>
+    <hyperlink ref="G5" r:id="rId14"/>
+    <hyperlink ref="G35" r:id="rId15"/>
+    <hyperlink ref="G6" r:id="rId16"/>
+    <hyperlink ref="G36" r:id="rId17"/>
+    <hyperlink ref="G24" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId19"/>
@@ -1014,7 +1492,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,6 +1524,9 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>86</v>
+      </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
renaming @lvl.core to @lvl/front-end, in accordance with https://github.com/jonathanburrows/lavalav/issues/7
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="192">
   <si>
     <t>Name</t>
   </si>
@@ -675,6 +675,9 @@
   </si>
   <si>
     <t>Move the contents of lvl.TestWebSite to TestWebSite, so that it can be found more easily in alphabetical order.</t>
+  </si>
+  <si>
+    <t>Remove the custom dotnet runner, and replace it with the built in one, so that mantenance is decreased.</t>
   </si>
 </sst>
 </file>
@@ -1102,21 +1105,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B36" sqref="A36:XFD36"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="195.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="195.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
@@ -1139,7 +1142,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>53</v>
       </c>
@@ -1162,7 +1165,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" t="s">
         <v>39</v>
@@ -1183,7 +1186,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
         <v>40</v>
@@ -1204,7 +1207,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" t="s">
         <v>42</v>
@@ -1225,7 +1228,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" t="s">
         <v>46</v>
@@ -1246,7 +1249,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>89</v>
       </c>
@@ -1269,7 +1272,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="B8" t="s">
         <v>54</v>
@@ -1290,7 +1293,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="B9" t="s">
         <v>56</v>
@@ -1311,7 +1314,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" t="s">
         <v>57</v>
@@ -1332,7 +1335,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" t="s">
         <v>58</v>
@@ -1353,7 +1356,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" t="s">
         <v>68</v>
@@ -1374,7 +1377,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
       <c r="B13" t="s">
         <v>59</v>
@@ -1395,7 +1398,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="B14" t="s">
         <v>60</v>
@@ -1416,7 +1419,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" t="s">
         <v>61</v>
@@ -1437,7 +1440,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
         <v>81</v>
@@ -1458,7 +1461,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
       <c r="B17" t="s">
         <v>63</v>
@@ -1479,7 +1482,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" t="s">
         <v>64</v>
@@ -1500,7 +1503,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>116</v>
       </c>
@@ -1523,7 +1526,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6"/>
       <c r="B20" t="s">
         <v>65</v>
@@ -1544,7 +1547,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="6"/>
       <c r="B21" t="s">
         <v>66</v>
@@ -1565,7 +1568,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="6"/>
       <c r="B22" t="s">
         <v>113</v>
@@ -1586,7 +1589,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6"/>
       <c r="B23" t="s">
         <v>114</v>
@@ -1607,7 +1610,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6"/>
       <c r="B24" t="s">
         <v>90</v>
@@ -1628,7 +1631,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="6"/>
       <c r="B25" t="s">
         <v>92</v>
@@ -1649,7 +1652,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6"/>
       <c r="B26" t="s">
         <v>94</v>
@@ -1670,7 +1673,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="6"/>
       <c r="B27" t="s">
         <v>96</v>
@@ -1691,7 +1694,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="6"/>
       <c r="B28" t="s">
         <v>110</v>
@@ -1712,7 +1715,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="6"/>
       <c r="B29" t="s">
         <v>98</v>
@@ -1733,7 +1736,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="6"/>
       <c r="B30" t="s">
         <v>100</v>
@@ -1754,7 +1757,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="6"/>
       <c r="B31" t="s">
         <v>102</v>
@@ -1775,7 +1778,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="6"/>
       <c r="B32" t="s">
         <v>104</v>
@@ -1796,7 +1799,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="6"/>
       <c r="B33" t="s">
         <v>106</v>
@@ -1808,7 +1811,7 @@
         <v>86</v>
       </c>
       <c r="E33" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F33" t="s">
         <v>29</v>
@@ -1817,7 +1820,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="6"/>
       <c r="B34" t="s">
         <v>108</v>
@@ -1829,7 +1832,7 @@
         <v>86</v>
       </c>
       <c r="E34" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F34" t="s">
         <v>29</v>
@@ -1838,7 +1841,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="5" t="s">
         <v>161</v>
       </c>
@@ -1852,7 +1855,7 @@
         <v>86</v>
       </c>
       <c r="E35" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F35" t="s">
         <v>30</v>
@@ -1861,7 +1864,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="5"/>
       <c r="B36" t="s">
         <v>118</v>
@@ -1873,7 +1876,7 @@
         <v>86</v>
       </c>
       <c r="E36" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F36" t="s">
         <v>30</v>
@@ -1882,7 +1885,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5"/>
       <c r="B37" t="s">
         <v>163</v>
@@ -1894,7 +1897,7 @@
         <v>86</v>
       </c>
       <c r="E37" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F37" t="s">
         <v>30</v>
@@ -1903,7 +1906,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5"/>
       <c r="B38" t="s">
         <v>166</v>
@@ -1915,7 +1918,7 @@
         <v>86</v>
       </c>
       <c r="E38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="s">
         <v>30</v>
@@ -1924,7 +1927,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="5"/>
       <c r="B39" t="s">
         <v>168</v>
@@ -1945,7 +1948,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5"/>
       <c r="B40" t="s">
         <v>173</v>
@@ -1966,7 +1969,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
       <c r="B41" t="s">
         <v>171</v>
@@ -1987,7 +1990,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5"/>
       <c r="B42" t="s">
         <v>174</v>
@@ -2008,7 +2011,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="5"/>
       <c r="B43" t="s">
         <v>176</v>
@@ -2029,7 +2032,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="5"/>
       <c r="B44" t="s">
         <v>178</v>
@@ -2050,7 +2053,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="5"/>
       <c r="B45" t="s">
         <v>185</v>
@@ -2071,7 +2074,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="5"/>
       <c r="B46" t="s">
         <v>184</v>
@@ -2092,7 +2095,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5"/>
       <c r="B47" t="s">
         <v>183</v>
@@ -2113,7 +2116,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="5"/>
       <c r="B48" t="s">
         <v>187</v>
@@ -2134,7 +2137,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5"/>
       <c r="B49" t="s">
         <v>188</v>
@@ -2155,7 +2158,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5"/>
       <c r="B50" t="s">
         <v>188</v>
@@ -2176,7 +2179,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5"/>
       <c r="B51" t="s">
         <v>119</v>
@@ -2188,13 +2191,16 @@
         <v>86</v>
       </c>
       <c r="E51" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F51" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G51" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="5"/>
       <c r="B52" t="s">
         <v>120</v>
@@ -2212,7 +2218,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5"/>
       <c r="B53" t="s">
         <v>121</v>
@@ -2230,7 +2236,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="5"/>
       <c r="B54" t="s">
         <v>122</v>
@@ -2248,7 +2254,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="5"/>
       <c r="B55" t="s">
         <v>123</v>
@@ -2266,7 +2272,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="5"/>
       <c r="B56" t="s">
         <v>124</v>
@@ -2284,7 +2290,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5"/>
       <c r="B57" t="s">
         <v>125</v>
@@ -2302,7 +2308,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="5"/>
       <c r="B58" t="s">
         <v>126</v>
@@ -2320,7 +2326,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5"/>
       <c r="B59" t="s">
         <v>127</v>
@@ -2338,7 +2344,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="5"/>
       <c r="B60" t="s">
         <v>128</v>
@@ -2356,7 +2362,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="5"/>
       <c r="B61" t="s">
         <v>129</v>
@@ -2374,7 +2380,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="5"/>
       <c r="B62" t="s">
         <v>130</v>
@@ -2392,7 +2398,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="5"/>
       <c r="B63" t="s">
         <v>131</v>
@@ -2410,7 +2416,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="5"/>
       <c r="B64" t="s">
         <v>132</v>
@@ -2428,7 +2434,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="5"/>
       <c r="B65" t="s">
         <v>133</v>
@@ -2446,7 +2452,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="5"/>
       <c r="B66" t="s">
         <v>134</v>
@@ -2464,7 +2470,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="5"/>
       <c r="B67" t="s">
         <v>135</v>
@@ -2482,7 +2488,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="5"/>
       <c r="B68" t="s">
         <v>136</v>
@@ -2500,7 +2506,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5"/>
       <c r="B69" t="s">
         <v>137</v>
@@ -2518,7 +2524,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
         <v>140</v>
       </c>
@@ -2535,7 +2541,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
         <v>141</v>
       </c>
@@ -2552,7 +2558,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B72" t="s">
         <v>142</v>
       </c>
@@ -2569,7 +2575,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
         <v>144</v>
       </c>
@@ -2586,7 +2592,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
         <v>143</v>
       </c>
@@ -2603,7 +2609,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B75" t="s">
         <v>147</v>
       </c>
@@ -2620,7 +2626,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B76" t="s">
         <v>148</v>
       </c>
@@ -2637,7 +2643,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
         <v>149</v>
       </c>
@@ -2654,7 +2660,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
         <v>145</v>
       </c>
@@ -2671,7 +2677,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
         <v>146</v>
       </c>
@@ -2688,7 +2694,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
         <v>151</v>
       </c>
@@ -2705,7 +2711,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
         <v>152</v>
       </c>
@@ -2722,7 +2728,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B82" t="s">
         <v>150</v>
       </c>
@@ -2739,7 +2745,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B83" t="s">
         <v>62</v>
       </c>
@@ -2756,7 +2762,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
         <v>153</v>
       </c>
@@ -2773,7 +2779,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
         <v>154</v>
       </c>
@@ -2790,7 +2796,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B86" t="s">
         <v>155</v>
       </c>
@@ -2807,7 +2813,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B87" t="s">
         <v>158</v>
       </c>
@@ -2824,7 +2830,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B88" t="s">
         <v>156</v>
       </c>
@@ -2841,7 +2847,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B89" t="s">
         <v>157</v>
       </c>
@@ -2858,7 +2864,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B90" t="s">
         <v>159</v>
       </c>
@@ -2875,7 +2881,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B91" t="s">
         <v>160</v>
       </c>
@@ -2892,7 +2898,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B92" t="s">
         <v>51</v>
       </c>
@@ -2912,7 +2918,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B93" t="s">
         <v>14</v>
       </c>
@@ -2932,7 +2938,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B94" t="s">
         <v>13</v>
       </c>
@@ -2952,7 +2958,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B95" t="s">
         <v>1</v>
       </c>
@@ -2972,7 +2978,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B96" t="s">
         <v>18</v>
       </c>
@@ -2992,7 +2998,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B97" t="s">
         <v>22</v>
       </c>
@@ -3012,7 +3018,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B98" t="s">
         <v>21</v>
       </c>
@@ -3032,7 +3038,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B99" t="s">
         <v>23</v>
       </c>
@@ -3052,7 +3058,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B100" t="s">
         <v>25</v>
       </c>
@@ -3072,7 +3078,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B101" t="s">
         <v>37</v>
       </c>
@@ -3092,7 +3098,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B102" t="s">
         <v>34</v>
       </c>
@@ -3112,7 +3118,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B103" t="s">
         <v>45</v>
       </c>
@@ -3132,7 +3138,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B104" t="s">
         <v>48</v>
       </c>
@@ -3152,7 +3158,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B105" t="s">
         <v>67</v>
       </c>
@@ -3172,7 +3178,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B106" t="s">
         <v>55</v>
       </c>
@@ -3199,7 +3205,7 @@
     <mergeCell ref="A35:A69"/>
     <mergeCell ref="A19:A34"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="3">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2 D4:D27 D98:D106 D109:D1048576 D29:D96">
       <formula1>Types</formula1>
     </dataValidation>
@@ -3243,13 +3249,13 @@
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -3260,7 +3266,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3271,7 +3277,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -3282,7 +3288,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -3290,7 +3296,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -3298,7 +3304,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
renaming @lvl.typescript-generator to TypeScriptGenerator, in accordance with https://github.com/jonathanburrows/lavalav/issues/8
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -1106,7 +1106,7 @@
   <dimension ref="A1:G106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1918,7 +1918,7 @@
         <v>86</v>
       </c>
       <c r="E38" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F38" t="s">
         <v>30</v>
@@ -2170,7 +2170,7 @@
         <v>86</v>
       </c>
       <c r="E50" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F50" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
renaming @lvl.typescript-generator.Tests to TypeScriptGenerator.Tests, in accordance with https://github.com/jonathanburrows/lavalav/issues/9
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -1106,7 +1106,7 @@
   <dimension ref="A1:G106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1939,7 +1939,7 @@
         <v>86</v>
       </c>
       <c r="E39" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F39" t="s">
         <v>30</v>
@@ -1960,7 +1960,7 @@
         <v>86</v>
       </c>
       <c r="E40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F40" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
moving all business agnostic projects to a core solution folder, in accordance with https://github.com/jonathanburrows/lavalav/issues/21
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="194">
   <si>
     <t>Name</t>
   </si>
@@ -678,6 +678,12 @@
   </si>
   <si>
     <t>Remove the custom dotnet runner, and replace it with the built in one, so that mantenance is decreased.</t>
+  </si>
+  <si>
+    <t>Create Core Solution folder</t>
+  </si>
+  <si>
+    <t>Move all projects which are agnostic to a business process to a core solution folder, so that projects can be grouped by business process later.</t>
   </si>
 </sst>
 </file>
@@ -1103,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G106"/>
+  <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="D35" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2182,7 +2188,7 @@
     <row r="51" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5"/>
       <c r="B51" t="s">
-        <v>119</v>
+        <v>192</v>
       </c>
       <c r="C51">
         <v>0.5</v>
@@ -2191,37 +2197,40 @@
         <v>86</v>
       </c>
       <c r="E51" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F51" t="s">
         <v>30</v>
       </c>
       <c r="G51" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="5"/>
       <c r="B52" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D52" t="s">
         <v>86</v>
       </c>
       <c r="E52" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F52" t="s">
         <v>30</v>
+      </c>
+      <c r="G52" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5"/>
       <c r="B53" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -2239,10 +2248,10 @@
     <row r="54" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="5"/>
       <c r="B54" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D54" t="s">
         <v>86</v>
@@ -2257,10 +2266,10 @@
     <row r="55" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="5"/>
       <c r="B55" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C55">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D55" t="s">
         <v>86</v>
@@ -2275,7 +2284,7 @@
     <row r="56" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="5"/>
       <c r="B56" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C56">
         <v>2</v>
@@ -2293,10 +2302,10 @@
     <row r="57" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5"/>
       <c r="B57" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C57">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D57" t="s">
         <v>86</v>
@@ -2311,10 +2320,10 @@
     <row r="58" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="5"/>
       <c r="B58" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C58">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D58" t="s">
         <v>86</v>
@@ -2329,7 +2338,7 @@
     <row r="59" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5"/>
       <c r="B59" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C59">
         <v>2</v>
@@ -2347,10 +2356,10 @@
     <row r="60" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="5"/>
       <c r="B60" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D60" t="s">
         <v>86</v>
@@ -2365,10 +2374,10 @@
     <row r="61" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="5"/>
       <c r="B61" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D61" t="s">
         <v>86</v>
@@ -2377,16 +2386,16 @@
         <v>9</v>
       </c>
       <c r="F61" t="s">
-        <v>139</v>
+        <v>30</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="5"/>
       <c r="B62" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D62" t="s">
         <v>86</v>
@@ -2395,13 +2404,13 @@
         <v>9</v>
       </c>
       <c r="F62" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="5"/>
       <c r="B63" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -2413,13 +2422,13 @@
         <v>9</v>
       </c>
       <c r="F63" t="s">
-        <v>30</v>
+        <v>138</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="5"/>
       <c r="B64" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -2431,13 +2440,13 @@
         <v>9</v>
       </c>
       <c r="F64" t="s">
-        <v>139</v>
+        <v>30</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="5"/>
       <c r="B65" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -2449,13 +2458,13 @@
         <v>9</v>
       </c>
       <c r="F65" t="s">
-        <v>29</v>
+        <v>139</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="5"/>
       <c r="B66" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -2467,16 +2476,16 @@
         <v>9</v>
       </c>
       <c r="F66" t="s">
-        <v>139</v>
+        <v>29</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="5"/>
       <c r="B67" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C67">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D67" t="s">
         <v>86</v>
@@ -2491,10 +2500,10 @@
     <row r="68" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="5"/>
       <c r="B68" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C68">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D68" t="s">
         <v>86</v>
@@ -2503,50 +2512,51 @@
         <v>9</v>
       </c>
       <c r="F68" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5"/>
       <c r="B69" t="s">
+        <v>136</v>
+      </c>
+      <c r="C69">
+        <v>2</v>
+      </c>
+      <c r="D69" t="s">
+        <v>86</v>
+      </c>
+      <c r="E69" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="5"/>
+      <c r="B70" t="s">
         <v>137</v>
       </c>
-      <c r="C69">
+      <c r="C70">
         <v>3</v>
       </c>
-      <c r="D69" t="s">
-        <v>86</v>
-      </c>
-      <c r="E69" t="s">
-        <v>9</v>
-      </c>
-      <c r="F69" t="s">
+      <c r="D70" t="s">
+        <v>86</v>
+      </c>
+      <c r="E70" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B70" t="s">
-        <v>140</v>
-      </c>
-      <c r="C70">
-        <v>2</v>
-      </c>
-      <c r="D70" t="s">
-        <v>86</v>
-      </c>
-      <c r="E70" t="s">
-        <v>9</v>
-      </c>
-      <c r="F70" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C71">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D71" t="s">
         <v>86</v>
@@ -2560,10 +2570,10 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B72" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C72">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D72" t="s">
         <v>86</v>
@@ -2577,10 +2587,10 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C73">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D73" t="s">
         <v>86</v>
@@ -2594,7 +2604,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -2611,10 +2621,10 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B75" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C75">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D75" t="s">
         <v>86</v>
@@ -2628,10 +2638,10 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B76" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C76">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D76" t="s">
         <v>86</v>
@@ -2645,7 +2655,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -2662,7 +2672,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -2679,10 +2689,10 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C79">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D79" t="s">
         <v>86</v>
@@ -2696,7 +2706,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C80">
         <v>2</v>
@@ -2713,7 +2723,7 @@
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C81">
         <v>2</v>
@@ -2730,10 +2740,10 @@
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B82" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C82">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D82" t="s">
         <v>86</v>
@@ -2747,7 +2757,7 @@
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B83" t="s">
-        <v>62</v>
+        <v>150</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -2764,10 +2774,10 @@
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
-        <v>153</v>
+        <v>62</v>
       </c>
       <c r="C84">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2781,10 +2791,10 @@
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C85">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D85" t="s">
         <v>86</v>
@@ -2798,10 +2808,10 @@
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B86" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C86">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D86" t="s">
         <v>86</v>
@@ -2815,10 +2825,10 @@
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B87" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C87">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D87" t="s">
         <v>86</v>
@@ -2832,10 +2842,10 @@
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B88" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C88">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D88" t="s">
         <v>86</v>
@@ -2849,10 +2859,10 @@
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B89" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C89">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D89" t="s">
         <v>86</v>
@@ -2866,7 +2876,7 @@
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B90" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C90">
         <v>2</v>
@@ -2883,10 +2893,10 @@
     </row>
     <row r="91" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B91" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C91">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D91" t="s">
         <v>86</v>
@@ -2900,30 +2910,27 @@
     </row>
     <row r="92" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B92" t="s">
-        <v>51</v>
+        <v>160</v>
       </c>
       <c r="C92">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D92" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="E92" t="s">
         <v>9</v>
       </c>
       <c r="F92" t="s">
         <v>29</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="93" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B93" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="C93">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D93" t="s">
         <v>2</v>
@@ -2932,15 +2939,15 @@
         <v>9</v>
       </c>
       <c r="F93" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
     </row>
     <row r="94" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B94" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C94">
         <v>1</v>
@@ -2955,15 +2962,15 @@
         <v>31</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="95" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B95" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C95">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D95" t="s">
         <v>2</v>
@@ -2975,15 +2982,15 @@
         <v>31</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="96" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B96" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C96">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D96" t="s">
         <v>2</v>
@@ -2995,15 +3002,15 @@
         <v>31</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="97" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B97" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C97">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D97" t="s">
         <v>2</v>
@@ -3015,15 +3022,15 @@
         <v>31</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B98" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C98">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D98" t="s">
         <v>2</v>
@@ -3035,15 +3042,15 @@
         <v>31</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B99" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C99">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D99" t="s">
         <v>2</v>
@@ -3055,12 +3062,12 @@
         <v>31</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="100" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B100" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C100">
         <v>1</v>
@@ -3075,35 +3082,35 @@
         <v>31</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="101" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B101" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C101">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D101" t="s">
         <v>2</v>
       </c>
       <c r="E101" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F101" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="102" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B102" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C102">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D102" t="s">
         <v>2</v>
@@ -3115,15 +3122,15 @@
         <v>29</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="103" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B103" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C103">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D103" t="s">
         <v>2</v>
@@ -3135,15 +3142,15 @@
         <v>29</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="104" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B104" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C104">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D104" t="s">
         <v>2</v>
@@ -3155,15 +3162,15 @@
         <v>29</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B105" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="C105">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D105" t="s">
         <v>2</v>
@@ -3174,13 +3181,13 @@
       <c r="F105" t="s">
         <v>29</v>
       </c>
-      <c r="G105" t="s">
-        <v>85</v>
+      <c r="G105" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B106" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="C106">
         <v>1</v>
@@ -3195,6 +3202,26 @@
         <v>29</v>
       </c>
       <c r="G106" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="107" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B107" t="s">
+        <v>55</v>
+      </c>
+      <c r="C107">
+        <v>1</v>
+      </c>
+      <c r="D107" t="s">
+        <v>2</v>
+      </c>
+      <c r="E107" t="s">
+        <v>12</v>
+      </c>
+      <c r="F107" t="s">
+        <v>29</v>
+      </c>
+      <c r="G107" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3202,39 +3229,39 @@
   <mergeCells count="4">
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A18"/>
-    <mergeCell ref="A35:A69"/>
+    <mergeCell ref="A35:A70"/>
     <mergeCell ref="A19:A34"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2 D4:D27 D98:D106 D109:D1048576 D29:D96">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2 D4:D27 D99:D107 D110:D1048576 D29:D97">
       <formula1>Types</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E98:E106 E109:E1048576 E2:E96">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E99:E107 E110:E1048576 E2:E97">
       <formula1>Statuses</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 F4:F27 F109:F1048576 F29:F106">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 F4:F27 F110:F1048576 F29:F107">
       <formula1>Themes</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G93" r:id="rId1"/>
-    <hyperlink ref="G95" r:id="rId2"/>
-    <hyperlink ref="G94" r:id="rId3"/>
-    <hyperlink ref="G96" r:id="rId4"/>
-    <hyperlink ref="G98" r:id="rId5"/>
-    <hyperlink ref="G97" r:id="rId6"/>
-    <hyperlink ref="G99" r:id="rId7"/>
-    <hyperlink ref="G100" r:id="rId8"/>
+    <hyperlink ref="G94" r:id="rId1"/>
+    <hyperlink ref="G96" r:id="rId2"/>
+    <hyperlink ref="G95" r:id="rId3"/>
+    <hyperlink ref="G97" r:id="rId4"/>
+    <hyperlink ref="G99" r:id="rId5"/>
+    <hyperlink ref="G98" r:id="rId6"/>
+    <hyperlink ref="G100" r:id="rId7"/>
+    <hyperlink ref="G101" r:id="rId8"/>
     <hyperlink ref="G2" r:id="rId9"/>
-    <hyperlink ref="G102" r:id="rId10"/>
-    <hyperlink ref="G101" r:id="rId11"/>
+    <hyperlink ref="G103" r:id="rId10"/>
+    <hyperlink ref="G102" r:id="rId11"/>
     <hyperlink ref="G3" r:id="rId12"/>
     <hyperlink ref="G4" r:id="rId13"/>
     <hyperlink ref="G5" r:id="rId14"/>
-    <hyperlink ref="G103" r:id="rId15"/>
+    <hyperlink ref="G104" r:id="rId15"/>
     <hyperlink ref="G6" r:id="rId16"/>
-    <hyperlink ref="G104" r:id="rId17"/>
-    <hyperlink ref="G92" r:id="rId18"/>
+    <hyperlink ref="G105" r:id="rId17"/>
+    <hyperlink ref="G93" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId19"/>

</xml_diff>

<commit_message>
renaming projects to remove prefix, in accordance with: https://github.com/jonathanburrows/lavalav/issues/10 https://github.com/jonathanburrows/lavalav/issues/11 https://github.com/jonathanburrows/lavalav/issues/12 https://github.com/jonathanburrows/lavalav/issues/13 https://github.com/jonathanburrows/lavalav/issues/14 https://github.com/jonathanburrows/lavalav/issues/15 https://github.com/jonathanburrows/lavalav/issues/16 https://github.com/jonathanburrows/lavalav/issues/17 https://github.com/jonathanburrows/lavalav/issues/18 https://github.com/jonathanburrows/lavalav/issues/19
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -1112,7 +1112,7 @@
   <dimension ref="A1:G107"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D35" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1966,7 +1966,7 @@
         <v>86</v>
       </c>
       <c r="E40" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F40" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Fixed concurrent SQLite bug, in accordance with https://github.com/jonathanburrows/lavalav/issues/22
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="195">
   <si>
     <t>Name</t>
   </si>
@@ -684,6 +684,9 @@
   </si>
   <si>
     <t>Move all projects which are agnostic to a business process to a core solution folder, so that projects can be grouped by business process later.</t>
+  </si>
+  <si>
+    <t>In the repository, insides transactions; add a lock to the transactions, so that asynchronous SQLite operations don’t end transactions before complete.</t>
   </si>
 </sst>
 </file>
@@ -1111,8 +1114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D35" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="G47" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1987,7 +1990,7 @@
         <v>86</v>
       </c>
       <c r="E41" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F41" t="s">
         <v>30</v>
@@ -2008,7 +2011,7 @@
         <v>86</v>
       </c>
       <c r="E42" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F42" t="s">
         <v>30</v>
@@ -2029,7 +2032,7 @@
         <v>86</v>
       </c>
       <c r="E43" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F43" t="s">
         <v>30</v>
@@ -2050,7 +2053,7 @@
         <v>86</v>
       </c>
       <c r="E44" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F44" t="s">
         <v>30</v>
@@ -2071,7 +2074,7 @@
         <v>86</v>
       </c>
       <c r="E45" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F45" t="s">
         <v>30</v>
@@ -2092,7 +2095,7 @@
         <v>86</v>
       </c>
       <c r="E46" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F46" t="s">
         <v>30</v>
@@ -2113,7 +2116,7 @@
         <v>86</v>
       </c>
       <c r="E47" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F47" t="s">
         <v>30</v>
@@ -2134,7 +2137,7 @@
         <v>86</v>
       </c>
       <c r="E48" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F48" t="s">
         <v>30</v>
@@ -2155,7 +2158,7 @@
         <v>86</v>
       </c>
       <c r="E49" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F49" t="s">
         <v>30</v>
@@ -2197,7 +2200,7 @@
         <v>86</v>
       </c>
       <c r="E51" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F51" t="s">
         <v>30</v>
@@ -2233,7 +2236,7 @@
         <v>120</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D53" t="s">
         <v>86</v>
@@ -2243,6 +2246,9 @@
       </c>
       <c r="F53" t="s">
         <v>30</v>
+      </c>
+      <c r="G53" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2251,7 +2257,7 @@
         <v>121</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D54" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
fixing assembly loader for executables, in accordance with https://github.com/jonathanburrows/lavalav/issues/23
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="196">
   <si>
     <t>Name</t>
   </si>
@@ -687,6 +687,9 @@
   </si>
   <si>
     <t>In the repository, insides transactions; add a lock to the transactions, so that asynchronous SQLite operations don’t end transactions before complete.</t>
+  </si>
+  <si>
+    <t>Allow the assembly loader to load executables, so that libraries can be loaded as well.</t>
   </si>
 </sst>
 </file>
@@ -1114,8 +1117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G47" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2242,7 +2245,7 @@
         <v>86</v>
       </c>
       <c r="E53" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F53" t="s">
         <v>30</v>
@@ -2263,10 +2266,13 @@
         <v>86</v>
       </c>
       <c r="E54" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" t="s">
         <v>30</v>
+      </c>
+      <c r="G54" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Modifying option objects names to be consistent, in accordance with https://github.com/jonathanburrows/lavalav/issues/24
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="207">
   <si>
     <t>Name</t>
   </si>
@@ -386,9 +386,6 @@
   </si>
   <si>
     <t>Assembly Loader Bug Fixes</t>
-  </si>
-  <si>
-    <t>Configuration Cleanup</t>
   </si>
   <si>
     <t>Console Logging</t>
@@ -690,6 +687,42 @@
   </si>
   <si>
     <t>Allow the assembly loader to load executables, so that libraries can be loaded as well.</t>
+  </si>
+  <si>
+    <t>Consistent Naming for Options Objects</t>
+  </si>
+  <si>
+    <t>For all configuration objects, make sure they are consistently named, and have the suffix Options.</t>
+  </si>
+  <si>
+    <t>Add Constructors for Options Objects</t>
+  </si>
+  <si>
+    <t>For all configuration objects, make sure they have both a parameterless constructor, and a constructor which accepts an IConfiguration.</t>
+  </si>
+  <si>
+    <t>Add Unit Tests for Options Binding</t>
+  </si>
+  <si>
+    <t>Add unit tests for the binding of configurations to options, so that binding to different types will be supported.</t>
+  </si>
+  <si>
+    <t>Change Options Objects Namespace</t>
+  </si>
+  <si>
+    <t>Change all Options object's namespaces to Microsoft.Extensions.DependencyInjection, so they are consistent with standards, and it has same namespace as IServiceCollectionExtensions.</t>
+  </si>
+  <si>
+    <t>Remove Options from MvcBuilderExtensions</t>
+  </si>
+  <si>
+    <t>Remove the WebOptions from the WebMvcBuilderExtensions methods, and read it from the ApplicationServices instead, so that duplicate code is removed.</t>
+  </si>
+  <si>
+    <t>Replace connectionString with DomainOptions</t>
+  </si>
+  <si>
+    <t>Replace the DomainExtensions.AddDomain connectionString parameter with a DomainOptions object, so that it can be read from the ServiceProvider.</t>
   </si>
 </sst>
 </file>
@@ -1115,10 +1148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G107"/>
+  <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="C35" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1855,7 +1888,7 @@
     </row>
     <row r="35" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B35" t="s">
         <v>117</v>
@@ -1873,7 +1906,7 @@
         <v>30</v>
       </c>
       <c r="G35" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -1894,13 +1927,13 @@
         <v>30</v>
       </c>
       <c r="G36" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5"/>
       <c r="B37" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C37">
         <v>0.5</v>
@@ -1915,13 +1948,13 @@
         <v>30</v>
       </c>
       <c r="G37" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5"/>
       <c r="B38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C38">
         <v>0.5</v>
@@ -1936,13 +1969,13 @@
         <v>30</v>
       </c>
       <c r="G38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="5"/>
       <c r="B39" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C39">
         <v>0.5</v>
@@ -1957,13 +1990,13 @@
         <v>30</v>
       </c>
       <c r="G39" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5"/>
       <c r="B40" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C40">
         <v>0.5</v>
@@ -1978,13 +2011,13 @@
         <v>30</v>
       </c>
       <c r="G40" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
       <c r="B41" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C41">
         <v>0.5</v>
@@ -1999,13 +2032,13 @@
         <v>30</v>
       </c>
       <c r="G41" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5"/>
       <c r="B42" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C42">
         <v>0.5</v>
@@ -2020,13 +2053,13 @@
         <v>30</v>
       </c>
       <c r="G42" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="5"/>
       <c r="B43" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C43">
         <v>0.5</v>
@@ -2041,13 +2074,13 @@
         <v>30</v>
       </c>
       <c r="G43" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="5"/>
       <c r="B44" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C44">
         <v>0.5</v>
@@ -2062,13 +2095,13 @@
         <v>30</v>
       </c>
       <c r="G44" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="5"/>
       <c r="B45" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C45">
         <v>0.5</v>
@@ -2083,13 +2116,13 @@
         <v>30</v>
       </c>
       <c r="G45" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="5"/>
       <c r="B46" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C46">
         <v>0.5</v>
@@ -2104,13 +2137,13 @@
         <v>30</v>
       </c>
       <c r="G46" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5"/>
       <c r="B47" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C47">
         <v>0.5</v>
@@ -2125,13 +2158,13 @@
         <v>30</v>
       </c>
       <c r="G47" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="5"/>
       <c r="B48" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C48">
         <v>0.5</v>
@@ -2146,13 +2179,13 @@
         <v>30</v>
       </c>
       <c r="G48" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5"/>
       <c r="B49" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C49">
         <v>0.5</v>
@@ -2167,13 +2200,13 @@
         <v>30</v>
       </c>
       <c r="G49" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5"/>
       <c r="B50" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C50">
         <v>0.5</v>
@@ -2188,13 +2221,13 @@
         <v>30</v>
       </c>
       <c r="G50" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5"/>
       <c r="B51" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C51">
         <v>0.5</v>
@@ -2209,7 +2242,7 @@
         <v>30</v>
       </c>
       <c r="G51" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2230,7 +2263,7 @@
         <v>30</v>
       </c>
       <c r="G52" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2251,7 +2284,7 @@
         <v>30</v>
       </c>
       <c r="G53" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2266,58 +2299,64 @@
         <v>86</v>
       </c>
       <c r="E54" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F54" t="s">
         <v>30</v>
       </c>
       <c r="G54" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="5"/>
       <c r="B55" t="s">
-        <v>122</v>
+        <v>195</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D55" t="s">
         <v>86</v>
       </c>
       <c r="E55" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" t="s">
         <v>30</v>
+      </c>
+      <c r="G55" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="5"/>
       <c r="B56" t="s">
-        <v>123</v>
+        <v>197</v>
       </c>
       <c r="C56">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="D56" t="s">
         <v>86</v>
       </c>
       <c r="E56" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" t="s">
         <v>30</v>
+      </c>
+      <c r="G56" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5"/>
       <c r="B57" t="s">
-        <v>124</v>
+        <v>199</v>
       </c>
       <c r="C57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D57" t="s">
         <v>86</v>
@@ -2327,15 +2366,18 @@
       </c>
       <c r="F57" t="s">
         <v>30</v>
+      </c>
+      <c r="G57" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="5"/>
       <c r="B58" t="s">
-        <v>125</v>
+        <v>201</v>
       </c>
       <c r="C58">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="D58" t="s">
         <v>86</v>
@@ -2345,15 +2387,18 @@
       </c>
       <c r="F58" t="s">
         <v>30</v>
+      </c>
+      <c r="G58" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5"/>
       <c r="B59" t="s">
-        <v>126</v>
+        <v>203</v>
       </c>
       <c r="C59">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="D59" t="s">
         <v>86</v>
@@ -2363,15 +2408,18 @@
       </c>
       <c r="F59" t="s">
         <v>30</v>
+      </c>
+      <c r="G59" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="5"/>
       <c r="B60" t="s">
-        <v>127</v>
+        <v>205</v>
       </c>
       <c r="C60">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="D60" t="s">
         <v>86</v>
@@ -2381,15 +2429,18 @@
       </c>
       <c r="F60" t="s">
         <v>30</v>
+      </c>
+      <c r="G60" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="5"/>
       <c r="B61" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D61" t="s">
         <v>86</v>
@@ -2398,16 +2449,16 @@
         <v>9</v>
       </c>
       <c r="F61" t="s">
-        <v>30</v>
+        <v>138</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="5"/>
       <c r="B62" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D62" t="s">
         <v>86</v>
@@ -2416,16 +2467,16 @@
         <v>9</v>
       </c>
       <c r="F62" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="5"/>
       <c r="B63" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C63">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D63" t="s">
         <v>86</v>
@@ -2440,10 +2491,10 @@
     <row r="64" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="5"/>
       <c r="B64" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C64">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D64" t="s">
         <v>86</v>
@@ -2452,16 +2503,16 @@
         <v>9</v>
       </c>
       <c r="F64" t="s">
-        <v>30</v>
+        <v>138</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="5"/>
       <c r="B65" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C65">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D65" t="s">
         <v>86</v>
@@ -2470,13 +2521,13 @@
         <v>9</v>
       </c>
       <c r="F65" t="s">
-        <v>139</v>
+        <v>30</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="5"/>
       <c r="B66" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -2488,16 +2539,16 @@
         <v>9</v>
       </c>
       <c r="F66" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="5"/>
       <c r="B67" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D67" t="s">
         <v>86</v>
@@ -2506,16 +2557,16 @@
         <v>9</v>
       </c>
       <c r="F67" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="5"/>
       <c r="B68" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C68">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D68" t="s">
         <v>86</v>
@@ -2524,16 +2575,16 @@
         <v>9</v>
       </c>
       <c r="F68" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5"/>
       <c r="B69" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D69" t="s">
         <v>86</v>
@@ -2542,102 +2593,107 @@
         <v>9</v>
       </c>
       <c r="F69" t="s">
-        <v>138</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="5"/>
       <c r="B70" t="s">
+        <v>131</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70" t="s">
+        <v>86</v>
+      </c>
+      <c r="E70" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="5"/>
+      <c r="B71" t="s">
+        <v>132</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71" t="s">
+        <v>86</v>
+      </c>
+      <c r="E71" t="s">
+        <v>9</v>
+      </c>
+      <c r="F71" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="5"/>
+      <c r="B72" t="s">
+        <v>133</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="D72" t="s">
+        <v>86</v>
+      </c>
+      <c r="E72" t="s">
+        <v>9</v>
+      </c>
+      <c r="F72" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="5"/>
+      <c r="B73" t="s">
+        <v>134</v>
+      </c>
+      <c r="C73">
+        <v>5</v>
+      </c>
+      <c r="D73" t="s">
+        <v>86</v>
+      </c>
+      <c r="E73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F73" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="5"/>
+      <c r="B74" t="s">
+        <v>135</v>
+      </c>
+      <c r="C74">
+        <v>2</v>
+      </c>
+      <c r="D74" t="s">
+        <v>86</v>
+      </c>
+      <c r="E74" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" t="s">
         <v>137</v>
       </c>
-      <c r="C70">
+    </row>
+    <row r="75" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="5"/>
+      <c r="B75" t="s">
+        <v>136</v>
+      </c>
+      <c r="C75">
         <v>3</v>
       </c>
-      <c r="D70" t="s">
-        <v>86</v>
-      </c>
-      <c r="E70" t="s">
-        <v>9</v>
-      </c>
-      <c r="F70" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B71" t="s">
-        <v>140</v>
-      </c>
-      <c r="C71">
-        <v>2</v>
-      </c>
-      <c r="D71" t="s">
-        <v>86</v>
-      </c>
-      <c r="E71" t="s">
-        <v>9</v>
-      </c>
-      <c r="F71" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B72" t="s">
-        <v>141</v>
-      </c>
-      <c r="C72">
-        <v>3</v>
-      </c>
-      <c r="D72" t="s">
-        <v>86</v>
-      </c>
-      <c r="E72" t="s">
-        <v>9</v>
-      </c>
-      <c r="F72" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B73" t="s">
-        <v>142</v>
-      </c>
-      <c r="C73">
-        <v>2</v>
-      </c>
-      <c r="D73" t="s">
-        <v>86</v>
-      </c>
-      <c r="E73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F73" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B74" t="s">
-        <v>144</v>
-      </c>
-      <c r="C74">
-        <v>1</v>
-      </c>
-      <c r="D74" t="s">
-        <v>86</v>
-      </c>
-      <c r="E74" t="s">
-        <v>9</v>
-      </c>
-      <c r="F74" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B75" t="s">
-        <v>143</v>
-      </c>
-      <c r="C75">
-        <v>1</v>
-      </c>
       <c r="D75" t="s">
         <v>86</v>
       </c>
@@ -2645,15 +2701,15 @@
         <v>9</v>
       </c>
       <c r="F75" t="s">
-        <v>29</v>
+        <v>138</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B76" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C76">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D76" t="s">
         <v>86</v>
@@ -2667,10 +2723,10 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C77">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D77" t="s">
         <v>86</v>
@@ -2684,10 +2740,10 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C78">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D78" t="s">
         <v>86</v>
@@ -2701,7 +2757,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C79">
         <v>1</v>
@@ -2718,328 +2774,313 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
+        <v>142</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80" t="s">
+        <v>86</v>
+      </c>
+      <c r="E80" t="s">
+        <v>9</v>
+      </c>
+      <c r="F80" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B81" t="s">
         <v>146</v>
       </c>
-      <c r="C80">
-        <v>2</v>
-      </c>
-      <c r="D80" t="s">
-        <v>86</v>
-      </c>
-      <c r="E80" t="s">
-        <v>9</v>
-      </c>
-      <c r="F80" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B81" t="s">
+      <c r="C81">
+        <v>3</v>
+      </c>
+      <c r="D81" t="s">
+        <v>86</v>
+      </c>
+      <c r="E81" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B82" t="s">
+        <v>147</v>
+      </c>
+      <c r="C82">
+        <v>1</v>
+      </c>
+      <c r="D82" t="s">
+        <v>86</v>
+      </c>
+      <c r="E82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F82" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B83" t="s">
+        <v>148</v>
+      </c>
+      <c r="C83">
+        <v>1</v>
+      </c>
+      <c r="D83" t="s">
+        <v>86</v>
+      </c>
+      <c r="E83" t="s">
+        <v>9</v>
+      </c>
+      <c r="F83" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B84" t="s">
+        <v>144</v>
+      </c>
+      <c r="C84">
+        <v>1</v>
+      </c>
+      <c r="D84" t="s">
+        <v>86</v>
+      </c>
+      <c r="E84" t="s">
+        <v>9</v>
+      </c>
+      <c r="F84" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B85" t="s">
+        <v>145</v>
+      </c>
+      <c r="C85">
+        <v>2</v>
+      </c>
+      <c r="D85" t="s">
+        <v>86</v>
+      </c>
+      <c r="E85" t="s">
+        <v>9</v>
+      </c>
+      <c r="F85" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B86" t="s">
+        <v>150</v>
+      </c>
+      <c r="C86">
+        <v>2</v>
+      </c>
+      <c r="D86" t="s">
+        <v>86</v>
+      </c>
+      <c r="E86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F86" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B87" t="s">
         <v>151</v>
       </c>
-      <c r="C81">
-        <v>2</v>
-      </c>
-      <c r="D81" t="s">
-        <v>86</v>
-      </c>
-      <c r="E81" t="s">
-        <v>9</v>
-      </c>
-      <c r="F81" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B82" t="s">
+      <c r="C87">
+        <v>2</v>
+      </c>
+      <c r="D87" t="s">
+        <v>86</v>
+      </c>
+      <c r="E87" t="s">
+        <v>9</v>
+      </c>
+      <c r="F87" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B88" t="s">
+        <v>149</v>
+      </c>
+      <c r="C88">
+        <v>1</v>
+      </c>
+      <c r="D88" t="s">
+        <v>86</v>
+      </c>
+      <c r="E88" t="s">
+        <v>9</v>
+      </c>
+      <c r="F88" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B89" t="s">
+        <v>62</v>
+      </c>
+      <c r="C89">
+        <v>1</v>
+      </c>
+      <c r="D89" t="s">
+        <v>86</v>
+      </c>
+      <c r="E89" t="s">
+        <v>9</v>
+      </c>
+      <c r="F89" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B90" t="s">
         <v>152</v>
       </c>
-      <c r="C82">
-        <v>2</v>
-      </c>
-      <c r="D82" t="s">
-        <v>86</v>
-      </c>
-      <c r="E82" t="s">
-        <v>9</v>
-      </c>
-      <c r="F82" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B83" t="s">
-        <v>150</v>
-      </c>
-      <c r="C83">
-        <v>1</v>
-      </c>
-      <c r="D83" t="s">
-        <v>86</v>
-      </c>
-      <c r="E83" t="s">
-        <v>9</v>
-      </c>
-      <c r="F83" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B84" t="s">
-        <v>62</v>
-      </c>
-      <c r="C84">
-        <v>1</v>
-      </c>
-      <c r="D84" t="s">
-        <v>86</v>
-      </c>
-      <c r="E84" t="s">
-        <v>9</v>
-      </c>
-      <c r="F84" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B85" t="s">
+      <c r="C90">
+        <v>2</v>
+      </c>
+      <c r="D90" t="s">
+        <v>86</v>
+      </c>
+      <c r="E90" t="s">
+        <v>9</v>
+      </c>
+      <c r="F90" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B91" t="s">
         <v>153</v>
       </c>
-      <c r="C85">
-        <v>2</v>
-      </c>
-      <c r="D85" t="s">
-        <v>86</v>
-      </c>
-      <c r="E85" t="s">
-        <v>9</v>
-      </c>
-      <c r="F85" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B86" t="s">
+      <c r="C91">
+        <v>1</v>
+      </c>
+      <c r="D91" t="s">
+        <v>86</v>
+      </c>
+      <c r="E91" t="s">
+        <v>9</v>
+      </c>
+      <c r="F91" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B92" t="s">
         <v>154</v>
       </c>
-      <c r="C86">
-        <v>1</v>
-      </c>
-      <c r="D86" t="s">
-        <v>86</v>
-      </c>
-      <c r="E86" t="s">
-        <v>9</v>
-      </c>
-      <c r="F86" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B87" t="s">
+      <c r="C92">
+        <v>0.5</v>
+      </c>
+      <c r="D92" t="s">
+        <v>86</v>
+      </c>
+      <c r="E92" t="s">
+        <v>9</v>
+      </c>
+      <c r="F92" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B93" t="s">
+        <v>157</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+      <c r="D93" t="s">
+        <v>86</v>
+      </c>
+      <c r="E93" t="s">
+        <v>9</v>
+      </c>
+      <c r="F93" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B94" t="s">
         <v>155</v>
       </c>
-      <c r="C87">
-        <v>0.5</v>
-      </c>
-      <c r="D87" t="s">
-        <v>86</v>
-      </c>
-      <c r="E87" t="s">
-        <v>9</v>
-      </c>
-      <c r="F87" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B88" t="s">
+      <c r="C94">
+        <v>3</v>
+      </c>
+      <c r="D94" t="s">
+        <v>86</v>
+      </c>
+      <c r="E94" t="s">
+        <v>9</v>
+      </c>
+      <c r="F94" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B95" t="s">
+        <v>156</v>
+      </c>
+      <c r="C95">
+        <v>2</v>
+      </c>
+      <c r="D95" t="s">
+        <v>86</v>
+      </c>
+      <c r="E95" t="s">
+        <v>9</v>
+      </c>
+      <c r="F95" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B96" t="s">
         <v>158</v>
       </c>
-      <c r="C88">
-        <v>1</v>
-      </c>
-      <c r="D88" t="s">
-        <v>86</v>
-      </c>
-      <c r="E88" t="s">
-        <v>9</v>
-      </c>
-      <c r="F88" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B89" t="s">
-        <v>156</v>
-      </c>
-      <c r="C89">
-        <v>3</v>
-      </c>
-      <c r="D89" t="s">
-        <v>86</v>
-      </c>
-      <c r="E89" t="s">
-        <v>9</v>
-      </c>
-      <c r="F89" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B90" t="s">
-        <v>157</v>
-      </c>
-      <c r="C90">
-        <v>2</v>
-      </c>
-      <c r="D90" t="s">
-        <v>86</v>
-      </c>
-      <c r="E90" t="s">
-        <v>9</v>
-      </c>
-      <c r="F90" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B91" t="s">
-        <v>159</v>
-      </c>
-      <c r="C91">
-        <v>2</v>
-      </c>
-      <c r="D91" t="s">
-        <v>86</v>
-      </c>
-      <c r="E91" t="s">
-        <v>9</v>
-      </c>
-      <c r="F91" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B92" t="s">
-        <v>160</v>
-      </c>
-      <c r="C92">
-        <v>5</v>
-      </c>
-      <c r="D92" t="s">
-        <v>86</v>
-      </c>
-      <c r="E92" t="s">
-        <v>9</v>
-      </c>
-      <c r="F92" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B93" t="s">
-        <v>51</v>
-      </c>
-      <c r="C93">
-        <v>3</v>
-      </c>
-      <c r="D93" t="s">
-        <v>2</v>
-      </c>
-      <c r="E93" t="s">
-        <v>9</v>
-      </c>
-      <c r="F93" t="s">
-        <v>29</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B94" t="s">
-        <v>14</v>
-      </c>
-      <c r="C94">
-        <v>1</v>
-      </c>
-      <c r="D94" t="s">
-        <v>2</v>
-      </c>
-      <c r="E94" t="s">
-        <v>9</v>
-      </c>
-      <c r="F94" t="s">
-        <v>31</v>
-      </c>
-      <c r="G94" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B95" t="s">
-        <v>13</v>
-      </c>
-      <c r="C95">
-        <v>1</v>
-      </c>
-      <c r="D95" t="s">
-        <v>2</v>
-      </c>
-      <c r="E95" t="s">
-        <v>9</v>
-      </c>
-      <c r="F95" t="s">
-        <v>31</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B96" t="s">
-        <v>1</v>
-      </c>
       <c r="C96">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D96" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="E96" t="s">
         <v>9</v>
       </c>
       <c r="F96" t="s">
-        <v>31</v>
-      </c>
-      <c r="G96" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="97" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B97" t="s">
-        <v>18</v>
+        <v>159</v>
       </c>
       <c r="C97">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D97" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="E97" t="s">
         <v>9</v>
       </c>
       <c r="F97" t="s">
-        <v>31</v>
-      </c>
-      <c r="G97" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B98" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="C98">
         <v>3</v>
@@ -3051,18 +3092,18 @@
         <v>9</v>
       </c>
       <c r="F98" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B99" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C99">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D99" t="s">
         <v>2</v>
@@ -3074,12 +3115,12 @@
         <v>31</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="100" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B100" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C100">
         <v>1</v>
@@ -3094,15 +3135,15 @@
         <v>31</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="101" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B101" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C101">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D101" t="s">
         <v>2</v>
@@ -3114,32 +3155,32 @@
         <v>31</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="102" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B102" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="C102">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D102" t="s">
         <v>2</v>
       </c>
       <c r="E102" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F102" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="103" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B103" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C103">
         <v>3</v>
@@ -3148,18 +3189,18 @@
         <v>2</v>
       </c>
       <c r="E103" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F103" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="104" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B104" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="C104">
         <v>2</v>
@@ -3168,38 +3209,38 @@
         <v>2</v>
       </c>
       <c r="E104" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F104" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B105" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="C105">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D105" t="s">
         <v>2</v>
       </c>
       <c r="E105" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F105" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B106" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="C106">
         <v>1</v>
@@ -3208,21 +3249,21 @@
         <v>2</v>
       </c>
       <c r="E106" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F106" t="s">
-        <v>29</v>
-      </c>
-      <c r="G106" t="s">
-        <v>85</v>
+        <v>31</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B107" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="C107">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D107" t="s">
         <v>2</v>
@@ -3233,7 +3274,107 @@
       <c r="F107" t="s">
         <v>29</v>
       </c>
-      <c r="G107" t="s">
+      <c r="G107" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B108" t="s">
+        <v>34</v>
+      </c>
+      <c r="C108">
+        <v>3</v>
+      </c>
+      <c r="D108" t="s">
+        <v>2</v>
+      </c>
+      <c r="E108" t="s">
+        <v>12</v>
+      </c>
+      <c r="F108" t="s">
+        <v>29</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B109" t="s">
+        <v>45</v>
+      </c>
+      <c r="C109">
+        <v>2</v>
+      </c>
+      <c r="D109" t="s">
+        <v>2</v>
+      </c>
+      <c r="E109" t="s">
+        <v>12</v>
+      </c>
+      <c r="F109" t="s">
+        <v>29</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B110" t="s">
+        <v>48</v>
+      </c>
+      <c r="C110">
+        <v>3</v>
+      </c>
+      <c r="D110" t="s">
+        <v>2</v>
+      </c>
+      <c r="E110" t="s">
+        <v>12</v>
+      </c>
+      <c r="F110" t="s">
+        <v>29</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B111" t="s">
+        <v>67</v>
+      </c>
+      <c r="C111">
+        <v>1</v>
+      </c>
+      <c r="D111" t="s">
+        <v>2</v>
+      </c>
+      <c r="E111" t="s">
+        <v>12</v>
+      </c>
+      <c r="F111" t="s">
+        <v>29</v>
+      </c>
+      <c r="G111" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="112" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B112" t="s">
+        <v>55</v>
+      </c>
+      <c r="C112">
+        <v>1</v>
+      </c>
+      <c r="D112" t="s">
+        <v>2</v>
+      </c>
+      <c r="E112" t="s">
+        <v>12</v>
+      </c>
+      <c r="F112" t="s">
+        <v>29</v>
+      </c>
+      <c r="G112" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3241,39 +3382,39 @@
   <mergeCells count="4">
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A18"/>
-    <mergeCell ref="A35:A70"/>
+    <mergeCell ref="A35:A75"/>
     <mergeCell ref="A19:A34"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2 D4:D27 D99:D107 D110:D1048576 D29:D97">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2 D4:D27 D104:D112 D115:D1048576 D29:D102">
       <formula1>Types</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E99:E107 E110:E1048576 E2:E97">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E104:E112 E115:E1048576 E2:E102">
       <formula1>Statuses</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 F4:F27 F110:F1048576 F29:F107">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 F4:F27 F115:F1048576 F29:F112">
       <formula1>Themes</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G94" r:id="rId1"/>
-    <hyperlink ref="G96" r:id="rId2"/>
-    <hyperlink ref="G95" r:id="rId3"/>
-    <hyperlink ref="G97" r:id="rId4"/>
-    <hyperlink ref="G99" r:id="rId5"/>
-    <hyperlink ref="G98" r:id="rId6"/>
-    <hyperlink ref="G100" r:id="rId7"/>
-    <hyperlink ref="G101" r:id="rId8"/>
+    <hyperlink ref="G99" r:id="rId1"/>
+    <hyperlink ref="G101" r:id="rId2"/>
+    <hyperlink ref="G100" r:id="rId3"/>
+    <hyperlink ref="G102" r:id="rId4"/>
+    <hyperlink ref="G104" r:id="rId5"/>
+    <hyperlink ref="G103" r:id="rId6"/>
+    <hyperlink ref="G105" r:id="rId7"/>
+    <hyperlink ref="G106" r:id="rId8"/>
     <hyperlink ref="G2" r:id="rId9"/>
-    <hyperlink ref="G103" r:id="rId10"/>
-    <hyperlink ref="G102" r:id="rId11"/>
+    <hyperlink ref="G108" r:id="rId10"/>
+    <hyperlink ref="G107" r:id="rId11"/>
     <hyperlink ref="G3" r:id="rId12"/>
     <hyperlink ref="G4" r:id="rId13"/>
     <hyperlink ref="G5" r:id="rId14"/>
-    <hyperlink ref="G104" r:id="rId15"/>
+    <hyperlink ref="G109" r:id="rId15"/>
     <hyperlink ref="G6" r:id="rId16"/>
-    <hyperlink ref="G105" r:id="rId17"/>
-    <hyperlink ref="G93" r:id="rId18"/>
+    <hyperlink ref="G110" r:id="rId17"/>
+    <hyperlink ref="G98" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId19"/>
@@ -3340,7 +3481,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -3348,7 +3489,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding IConfiguration to constructors of Option objects, in accordance with https://github.com/jonathanburrows/lavalav/issues/25
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -1150,8 +1150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C35" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2320,7 +2320,7 @@
         <v>86</v>
       </c>
       <c r="E55" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F55" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
updating Options objects to have Microsoft.Extensions.DepdenecyInjection, in accordance with https://github.com/jonathanburrows/lavalav/issues/27
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -1151,7 +1151,7 @@
   <dimension ref="A1:G112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2341,7 +2341,7 @@
         <v>86</v>
       </c>
       <c r="E56" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F56" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
adding unit tests to option objects, in accordance with https://github.com/jonathanburrows/lavalav/issues/26
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -1150,8 +1150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="C26" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2383,7 +2383,7 @@
         <v>86</v>
       </c>
       <c r="E58" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F58" t="s">
         <v>30</v>
@@ -2404,7 +2404,7 @@
         <v>86</v>
       </c>
       <c r="E59" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F59" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
fixing SCA errors, and adding DomainOptions, in accordance with https://github.com/jonathanburrows/lavalav/issues/28
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -1150,8 +1150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C26" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="C29" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2362,7 +2362,7 @@
         <v>86</v>
       </c>
       <c r="E57" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F57" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
adding error messages to response and console window, in accordance with https://github.com/jonathanburrows/lavalav/issues/30 https://github.com/jonathanburrows/lavalav/issues/31
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="208">
   <si>
     <t>Name</t>
   </si>
@@ -723,6 +723,9 @@
   </si>
   <si>
     <t>Replace the DomainExtensions.AddDomain connectionString parameter with a DomainOptions object, so that it can be read from the ServiceProvider.</t>
+  </si>
+  <si>
+    <t>Add Database Escape Quotes</t>
   </si>
 </sst>
 </file>
@@ -819,10 +822,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1148,10 +1154,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G112"/>
+  <dimension ref="A1:G113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C29" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1188,7 +1194,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>53</v>
       </c>
       <c r="B2" t="s">
@@ -1211,7 +1217,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
+      <c r="A3" s="4"/>
       <c r="B3" t="s">
         <v>39</v>
       </c>
@@ -1232,7 +1238,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
+      <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>40</v>
       </c>
@@ -1253,7 +1259,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
+      <c r="A5" s="4"/>
       <c r="B5" t="s">
         <v>42</v>
       </c>
@@ -1274,7 +1280,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
+      <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>46</v>
       </c>
@@ -1295,7 +1301,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>89</v>
       </c>
       <c r="B7" t="s">
@@ -1318,7 +1324,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="4"/>
+      <c r="A8" s="5"/>
       <c r="B8" t="s">
         <v>54</v>
       </c>
@@ -1339,7 +1345,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4"/>
+      <c r="A9" s="5"/>
       <c r="B9" t="s">
         <v>56</v>
       </c>
@@ -1360,7 +1366,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4"/>
+      <c r="A10" s="5"/>
       <c r="B10" t="s">
         <v>57</v>
       </c>
@@ -1381,7 +1387,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4"/>
+      <c r="A11" s="5"/>
       <c r="B11" t="s">
         <v>58</v>
       </c>
@@ -1402,7 +1408,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4"/>
+      <c r="A12" s="5"/>
       <c r="B12" t="s">
         <v>68</v>
       </c>
@@ -1423,7 +1429,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
+      <c r="A13" s="5"/>
       <c r="B13" t="s">
         <v>59</v>
       </c>
@@ -1444,7 +1450,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="4"/>
+      <c r="A14" s="5"/>
       <c r="B14" t="s">
         <v>60</v>
       </c>
@@ -1465,7 +1471,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="4"/>
+      <c r="A15" s="5"/>
       <c r="B15" t="s">
         <v>61</v>
       </c>
@@ -1486,7 +1492,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
+      <c r="A16" s="5"/>
       <c r="B16" t="s">
         <v>81</v>
       </c>
@@ -1507,7 +1513,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="4"/>
+      <c r="A17" s="5"/>
       <c r="B17" t="s">
         <v>63</v>
       </c>
@@ -1528,7 +1534,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
+      <c r="A18" s="5"/>
       <c r="B18" t="s">
         <v>64</v>
       </c>
@@ -1549,7 +1555,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="7" t="s">
         <v>116</v>
       </c>
       <c r="B19" t="s">
@@ -1572,7 +1578,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="6"/>
+      <c r="A20" s="7"/>
       <c r="B20" t="s">
         <v>65</v>
       </c>
@@ -1593,7 +1599,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="6"/>
+      <c r="A21" s="7"/>
       <c r="B21" t="s">
         <v>66</v>
       </c>
@@ -1614,7 +1620,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="6"/>
+      <c r="A22" s="7"/>
       <c r="B22" t="s">
         <v>113</v>
       </c>
@@ -1635,7 +1641,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="6"/>
+      <c r="A23" s="7"/>
       <c r="B23" t="s">
         <v>114</v>
       </c>
@@ -1656,7 +1662,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="6"/>
+      <c r="A24" s="7"/>
       <c r="B24" t="s">
         <v>90</v>
       </c>
@@ -1677,7 +1683,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="6"/>
+      <c r="A25" s="7"/>
       <c r="B25" t="s">
         <v>92</v>
       </c>
@@ -1698,7 +1704,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="6"/>
+      <c r="A26" s="7"/>
       <c r="B26" t="s">
         <v>94</v>
       </c>
@@ -1719,7 +1725,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="6"/>
+      <c r="A27" s="7"/>
       <c r="B27" t="s">
         <v>96</v>
       </c>
@@ -1740,7 +1746,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="6"/>
+      <c r="A28" s="7"/>
       <c r="B28" t="s">
         <v>110</v>
       </c>
@@ -1761,7 +1767,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="6"/>
+      <c r="A29" s="7"/>
       <c r="B29" t="s">
         <v>98</v>
       </c>
@@ -1782,7 +1788,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="6"/>
+      <c r="A30" s="7"/>
       <c r="B30" t="s">
         <v>100</v>
       </c>
@@ -1803,7 +1809,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="6"/>
+      <c r="A31" s="7"/>
       <c r="B31" t="s">
         <v>102</v>
       </c>
@@ -1824,7 +1830,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="6"/>
+      <c r="A32" s="7"/>
       <c r="B32" t="s">
         <v>104</v>
       </c>
@@ -1845,7 +1851,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="6"/>
+      <c r="A33" s="7"/>
       <c r="B33" t="s">
         <v>106</v>
       </c>
@@ -1866,7 +1872,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="6"/>
+      <c r="A34" s="7"/>
       <c r="B34" t="s">
         <v>108</v>
       </c>
@@ -1887,7 +1893,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="6" t="s">
         <v>160</v>
       </c>
       <c r="B35" t="s">
@@ -1910,7 +1916,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="5"/>
+      <c r="A36" s="6"/>
       <c r="B36" t="s">
         <v>118</v>
       </c>
@@ -1931,7 +1937,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="5"/>
+      <c r="A37" s="6"/>
       <c r="B37" t="s">
         <v>162</v>
       </c>
@@ -1952,7 +1958,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="5"/>
+      <c r="A38" s="6"/>
       <c r="B38" t="s">
         <v>165</v>
       </c>
@@ -1973,7 +1979,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="5"/>
+      <c r="A39" s="6"/>
       <c r="B39" t="s">
         <v>167</v>
       </c>
@@ -1994,7 +2000,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="5"/>
+      <c r="A40" s="6"/>
       <c r="B40" t="s">
         <v>172</v>
       </c>
@@ -2015,7 +2021,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="5"/>
+      <c r="A41" s="6"/>
       <c r="B41" t="s">
         <v>170</v>
       </c>
@@ -2036,7 +2042,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="5"/>
+      <c r="A42" s="6"/>
       <c r="B42" t="s">
         <v>173</v>
       </c>
@@ -2057,7 +2063,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="5"/>
+      <c r="A43" s="6"/>
       <c r="B43" t="s">
         <v>175</v>
       </c>
@@ -2078,7 +2084,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="5"/>
+      <c r="A44" s="6"/>
       <c r="B44" t="s">
         <v>177</v>
       </c>
@@ -2099,7 +2105,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="5"/>
+      <c r="A45" s="6"/>
       <c r="B45" t="s">
         <v>184</v>
       </c>
@@ -2120,7 +2126,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="5"/>
+      <c r="A46" s="6"/>
       <c r="B46" t="s">
         <v>183</v>
       </c>
@@ -2141,7 +2147,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="5"/>
+      <c r="A47" s="6"/>
       <c r="B47" t="s">
         <v>182</v>
       </c>
@@ -2162,7 +2168,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="5"/>
+      <c r="A48" s="6"/>
       <c r="B48" t="s">
         <v>186</v>
       </c>
@@ -2183,7 +2189,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="5"/>
+      <c r="A49" s="6"/>
       <c r="B49" t="s">
         <v>187</v>
       </c>
@@ -2204,7 +2210,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="5"/>
+      <c r="A50" s="6"/>
       <c r="B50" t="s">
         <v>187</v>
       </c>
@@ -2225,7 +2231,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="5"/>
+      <c r="A51" s="6"/>
       <c r="B51" t="s">
         <v>191</v>
       </c>
@@ -2246,7 +2252,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="5"/>
+      <c r="A52" s="6"/>
       <c r="B52" t="s">
         <v>119</v>
       </c>
@@ -2267,7 +2273,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="5"/>
+      <c r="A53" s="6"/>
       <c r="B53" t="s">
         <v>120</v>
       </c>
@@ -2288,7 +2294,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="5"/>
+      <c r="A54" s="6"/>
       <c r="B54" t="s">
         <v>121</v>
       </c>
@@ -2309,7 +2315,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="5"/>
+      <c r="A55" s="6"/>
       <c r="B55" t="s">
         <v>195</v>
       </c>
@@ -2330,7 +2336,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="5"/>
+      <c r="A56" s="6"/>
       <c r="B56" t="s">
         <v>197</v>
       </c>
@@ -2351,7 +2357,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="5"/>
+      <c r="A57" s="6"/>
       <c r="B57" t="s">
         <v>199</v>
       </c>
@@ -2372,7 +2378,7 @@
       </c>
     </row>
     <row r="58" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="5"/>
+      <c r="A58" s="6"/>
       <c r="B58" t="s">
         <v>201</v>
       </c>
@@ -2393,7 +2399,7 @@
       </c>
     </row>
     <row r="59" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="5"/>
+      <c r="A59" s="6"/>
       <c r="B59" t="s">
         <v>203</v>
       </c>
@@ -2414,7 +2420,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="5"/>
+      <c r="A60" s="6"/>
       <c r="B60" t="s">
         <v>205</v>
       </c>
@@ -2435,7 +2441,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="5"/>
+      <c r="A61" s="6"/>
       <c r="B61" t="s">
         <v>122</v>
       </c>
@@ -2446,14 +2452,14 @@
         <v>86</v>
       </c>
       <c r="E61" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F61" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="5"/>
+      <c r="A62" s="6"/>
       <c r="B62" t="s">
         <v>123</v>
       </c>
@@ -2464,14 +2470,14 @@
         <v>86</v>
       </c>
       <c r="E62" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="5"/>
+      <c r="A63" s="6"/>
       <c r="B63" t="s">
         <v>124</v>
       </c>
@@ -2489,7 +2495,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="5"/>
+      <c r="A64" s="6"/>
       <c r="B64" t="s">
         <v>125</v>
       </c>
@@ -2507,7 +2513,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="5"/>
+      <c r="A65" s="6"/>
       <c r="B65" t="s">
         <v>126</v>
       </c>
@@ -2525,7 +2531,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="5"/>
+      <c r="A66" s="6"/>
       <c r="B66" t="s">
         <v>127</v>
       </c>
@@ -2543,7 +2549,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="5"/>
+      <c r="A67" s="6"/>
       <c r="B67" t="s">
         <v>128</v>
       </c>
@@ -2561,7 +2567,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="5"/>
+      <c r="A68" s="6"/>
       <c r="B68" t="s">
         <v>129</v>
       </c>
@@ -2579,7 +2585,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="5"/>
+      <c r="A69" s="6"/>
       <c r="B69" t="s">
         <v>130</v>
       </c>
@@ -2597,7 +2603,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="5"/>
+      <c r="A70" s="6"/>
       <c r="B70" t="s">
         <v>131</v>
       </c>
@@ -2615,7 +2621,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="5"/>
+      <c r="A71" s="6"/>
       <c r="B71" t="s">
         <v>132</v>
       </c>
@@ -2633,7 +2639,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="5"/>
+      <c r="A72" s="6"/>
       <c r="B72" t="s">
         <v>133</v>
       </c>
@@ -2651,7 +2657,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="5"/>
+      <c r="A73" s="6"/>
       <c r="B73" t="s">
         <v>134</v>
       </c>
@@ -2669,7 +2675,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="5"/>
+      <c r="A74" s="6"/>
       <c r="B74" t="s">
         <v>135</v>
       </c>
@@ -2687,7 +2693,7 @@
       </c>
     </row>
     <row r="75" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="5"/>
+      <c r="A75" s="6"/>
       <c r="B75" t="s">
         <v>136</v>
       </c>
@@ -2704,12 +2710,13 @@
         <v>138</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="3"/>
       <c r="B76" t="s">
-        <v>139</v>
+        <v>207</v>
       </c>
       <c r="C76">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D76" t="s">
         <v>86</v>
@@ -2718,15 +2725,15 @@
         <v>9</v>
       </c>
       <c r="F76" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C77">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D77" t="s">
         <v>86</v>
@@ -2740,10 +2747,10 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C78">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D78" t="s">
         <v>86</v>
@@ -2757,10 +2764,10 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C79">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D79" t="s">
         <v>86</v>
@@ -2774,7 +2781,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -2791,10 +2798,10 @@
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C81">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D81" t="s">
         <v>86</v>
@@ -2808,10 +2815,10 @@
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B82" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C82">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D82" t="s">
         <v>86</v>
@@ -2825,7 +2832,7 @@
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B83" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -2842,7 +2849,7 @@
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C84">
         <v>1</v>
@@ -2859,10 +2866,10 @@
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C85">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D85" t="s">
         <v>86</v>
@@ -2876,7 +2883,7 @@
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B86" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C86">
         <v>2</v>
@@ -2893,7 +2900,7 @@
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B87" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C87">
         <v>2</v>
@@ -2910,10 +2917,10 @@
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B88" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C88">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D88" t="s">
         <v>86</v>
@@ -2927,7 +2934,7 @@
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B89" t="s">
-        <v>62</v>
+        <v>149</v>
       </c>
       <c r="C89">
         <v>1</v>
@@ -2944,10 +2951,10 @@
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B90" t="s">
-        <v>152</v>
+        <v>62</v>
       </c>
       <c r="C90">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D90" t="s">
         <v>86</v>
@@ -2961,10 +2968,10 @@
     </row>
     <row r="91" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B91" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C91">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D91" t="s">
         <v>86</v>
@@ -2978,10 +2985,10 @@
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B92" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C92">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D92" t="s">
         <v>86</v>
@@ -2995,10 +3002,10 @@
     </row>
     <row r="93" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B93" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C93">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D93" t="s">
         <v>86</v>
@@ -3012,10 +3019,10 @@
     </row>
     <row r="94" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B94" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C94">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D94" t="s">
         <v>86</v>
@@ -3029,10 +3036,10 @@
     </row>
     <row r="95" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B95" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C95">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D95" t="s">
         <v>86</v>
@@ -3046,7 +3053,7 @@
     </row>
     <row r="96" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B96" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C96">
         <v>2</v>
@@ -3063,10 +3070,10 @@
     </row>
     <row r="97" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B97" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C97">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D97" t="s">
         <v>86</v>
@@ -3080,30 +3087,27 @@
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B98" t="s">
-        <v>51</v>
+        <v>159</v>
       </c>
       <c r="C98">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D98" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="E98" t="s">
         <v>9</v>
       </c>
       <c r="F98" t="s">
         <v>29</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B99" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="C99">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D99" t="s">
         <v>2</v>
@@ -3112,15 +3116,15 @@
         <v>9</v>
       </c>
       <c r="F99" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
     </row>
     <row r="100" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B100" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C100">
         <v>1</v>
@@ -3135,15 +3139,15 @@
         <v>31</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="101" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B101" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C101">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D101" t="s">
         <v>2</v>
@@ -3155,15 +3159,15 @@
         <v>31</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="102" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B102" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C102">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D102" t="s">
         <v>2</v>
@@ -3175,15 +3179,15 @@
         <v>31</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="103" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B103" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C103">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D103" t="s">
         <v>2</v>
@@ -3195,15 +3199,15 @@
         <v>31</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="104" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B104" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C104">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D104" t="s">
         <v>2</v>
@@ -3215,15 +3219,15 @@
         <v>31</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B105" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C105">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D105" t="s">
         <v>2</v>
@@ -3235,12 +3239,12 @@
         <v>31</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B106" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C106">
         <v>1</v>
@@ -3255,35 +3259,35 @@
         <v>31</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B107" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C107">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D107" t="s">
         <v>2</v>
       </c>
       <c r="E107" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F107" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="108" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B108" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C108">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D108" t="s">
         <v>2</v>
@@ -3295,15 +3299,15 @@
         <v>29</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="109" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B109" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C109">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D109" t="s">
         <v>2</v>
@@ -3315,15 +3319,15 @@
         <v>29</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="110" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B110" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C110">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D110" t="s">
         <v>2</v>
@@ -3335,15 +3339,15 @@
         <v>29</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="111" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B111" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="C111">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D111" t="s">
         <v>2</v>
@@ -3354,13 +3358,13 @@
       <c r="F111" t="s">
         <v>29</v>
       </c>
-      <c r="G111" t="s">
-        <v>85</v>
+      <c r="G111" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="112" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B112" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="C112">
         <v>1</v>
@@ -3375,6 +3379,26 @@
         <v>29</v>
       </c>
       <c r="G112" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="113" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B113" t="s">
+        <v>55</v>
+      </c>
+      <c r="C113">
+        <v>1</v>
+      </c>
+      <c r="D113" t="s">
+        <v>2</v>
+      </c>
+      <c r="E113" t="s">
+        <v>12</v>
+      </c>
+      <c r="F113" t="s">
+        <v>29</v>
+      </c>
+      <c r="G113" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3386,35 +3410,35 @@
     <mergeCell ref="A19:A34"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2 D4:D27 D104:D112 D115:D1048576 D29:D102">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2 D4:D27 D105:D113 D116:D1048576 D29:D103">
       <formula1>Types</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E104:E112 E115:E1048576 E2:E102">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E105:E113 E116:E1048576 E2:E103">
       <formula1>Statuses</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 F4:F27 F115:F1048576 F29:F112">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 F4:F27 F116:F1048576 F29:F113">
       <formula1>Themes</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G99" r:id="rId1"/>
-    <hyperlink ref="G101" r:id="rId2"/>
-    <hyperlink ref="G100" r:id="rId3"/>
-    <hyperlink ref="G102" r:id="rId4"/>
-    <hyperlink ref="G104" r:id="rId5"/>
-    <hyperlink ref="G103" r:id="rId6"/>
-    <hyperlink ref="G105" r:id="rId7"/>
-    <hyperlink ref="G106" r:id="rId8"/>
+    <hyperlink ref="G100" r:id="rId1"/>
+    <hyperlink ref="G102" r:id="rId2"/>
+    <hyperlink ref="G101" r:id="rId3"/>
+    <hyperlink ref="G103" r:id="rId4"/>
+    <hyperlink ref="G105" r:id="rId5"/>
+    <hyperlink ref="G104" r:id="rId6"/>
+    <hyperlink ref="G106" r:id="rId7"/>
+    <hyperlink ref="G107" r:id="rId8"/>
     <hyperlink ref="G2" r:id="rId9"/>
-    <hyperlink ref="G108" r:id="rId10"/>
-    <hyperlink ref="G107" r:id="rId11"/>
+    <hyperlink ref="G109" r:id="rId10"/>
+    <hyperlink ref="G108" r:id="rId11"/>
     <hyperlink ref="G3" r:id="rId12"/>
     <hyperlink ref="G4" r:id="rId13"/>
     <hyperlink ref="G5" r:id="rId14"/>
-    <hyperlink ref="G109" r:id="rId15"/>
+    <hyperlink ref="G110" r:id="rId15"/>
     <hyperlink ref="G6" r:id="rId16"/>
-    <hyperlink ref="G110" r:id="rId17"/>
-    <hyperlink ref="G98" r:id="rId18"/>
+    <hyperlink ref="G111" r:id="rId17"/>
+    <hyperlink ref="G99" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId19"/>

</xml_diff>

<commit_message>
added required convention, in accordance with https://github.com/jonathanburrows/lavalav/issues/32
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="211">
   <si>
     <t>Name</t>
   </si>
@@ -726,6 +726,15 @@
   </si>
   <si>
     <t>Add Database Escape Quotes</t>
+  </si>
+  <si>
+    <t>When an error occurs during a request, the error message should be attached to the response body, and the status code 500.</t>
+  </si>
+  <si>
+    <t>When the hosting environment is Development, then have the error messages also output to the console window.</t>
+  </si>
+  <si>
+    <t>Write a suite of attributes which will modify the mappings of an entity, so that mappings are centralised to the class they belong to.</t>
   </si>
 </sst>
 </file>
@@ -1156,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" topLeftCell="C40" workbookViewId="0">
+      <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2457,6 +2466,9 @@
       <c r="F61" t="s">
         <v>138</v>
       </c>
+      <c r="G61" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="62" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="6"/>
@@ -2470,10 +2482,13 @@
         <v>86</v>
       </c>
       <c r="E62" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F62" t="s">
         <v>138</v>
+      </c>
+      <c r="G62" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2488,10 +2503,13 @@
         <v>86</v>
       </c>
       <c r="E63" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" t="s">
         <v>138</v>
+      </c>
+      <c r="G63" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
added foreign key id convention, in accordance with https://github.com/jonathanburrows/lavalav/issues/32
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -1165,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C40" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2440,7 +2440,7 @@
         <v>86</v>
       </c>
       <c r="E60" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F60" t="s">
         <v>30</v>
@@ -2503,7 +2503,7 @@
         <v>86</v>
       </c>
       <c r="E63" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F63" t="s">
         <v>138</v>

</xml_diff>

<commit_message>
added an abstract entity base class, in accordance with https://github.com/jonathanburrows/lavalav/issues/33
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -12,7 +12,7 @@
   </sheets>
   <definedNames>
     <definedName name="Statuses">'drop-downs'!$B$2:$B$6</definedName>
-    <definedName name="Themes">'drop-downs'!$C$2:$C$6</definedName>
+    <definedName name="Themes">'drop-downs'!$C$2:$C$7</definedName>
     <definedName name="Types">'drop-downs'!$A$2:$A$3</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="219">
   <si>
     <t>Name</t>
   </si>
@@ -395,9 +395,6 @@
   </si>
   <si>
     <t>NHibernate Conventions</t>
-  </si>
-  <si>
-    <t>Aggregate Pattern</t>
   </si>
   <si>
     <t>Database Migration Refactoring</t>
@@ -735,6 +732,33 @@
   </si>
   <si>
     <t>Write a suite of attributes which will modify the mappings of an entity, so that mappings are centralised to the class they belong to.</t>
+  </si>
+  <si>
+    <t>Abstract Entity Class</t>
+  </si>
+  <si>
+    <t>Add an abstract class, Entity, which replaces the interface IEntity, so that comparisons between entities is simplified.</t>
+  </si>
+  <si>
+    <t>Add Aggregate Scopes</t>
+  </si>
+  <si>
+    <t>Introduce the concept of aggregate scopes, so that DDD concepts can be applied.</t>
+  </si>
+  <si>
+    <t>Replace Xunit with Fluent Assertions, so that natural language can be used to describe unit tests.</t>
+  </si>
+  <si>
+    <t>Replace Xunit with FluentAssertions</t>
+  </si>
+  <si>
+    <t>Investigate what SMWU would like, so that a proposal can be formed.</t>
+  </si>
+  <si>
+    <t>SMWU Due Code Investigation</t>
+  </si>
+  <si>
+    <t>SMWU</t>
   </si>
 </sst>
 </file>
@@ -1163,10 +1187,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G113"/>
+  <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1903,7 +1927,7 @@
     </row>
     <row r="35" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B35" t="s">
         <v>117</v>
@@ -1921,7 +1945,7 @@
         <v>30</v>
       </c>
       <c r="G35" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -1942,13 +1966,13 @@
         <v>30</v>
       </c>
       <c r="G36" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="6"/>
       <c r="B37" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C37">
         <v>0.5</v>
@@ -1963,13 +1987,13 @@
         <v>30</v>
       </c>
       <c r="G37" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="6"/>
       <c r="B38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C38">
         <v>0.5</v>
@@ -1984,13 +2008,13 @@
         <v>30</v>
       </c>
       <c r="G38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="6"/>
       <c r="B39" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C39">
         <v>0.5</v>
@@ -2005,13 +2029,13 @@
         <v>30</v>
       </c>
       <c r="G39" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="6"/>
       <c r="B40" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C40">
         <v>0.5</v>
@@ -2026,13 +2050,13 @@
         <v>30</v>
       </c>
       <c r="G40" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="6"/>
       <c r="B41" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C41">
         <v>0.5</v>
@@ -2047,13 +2071,13 @@
         <v>30</v>
       </c>
       <c r="G41" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="6"/>
       <c r="B42" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C42">
         <v>0.5</v>
@@ -2068,13 +2092,13 @@
         <v>30</v>
       </c>
       <c r="G42" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="6"/>
       <c r="B43" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C43">
         <v>0.5</v>
@@ -2089,13 +2113,13 @@
         <v>30</v>
       </c>
       <c r="G43" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="6"/>
       <c r="B44" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C44">
         <v>0.5</v>
@@ -2110,13 +2134,13 @@
         <v>30</v>
       </c>
       <c r="G44" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="6"/>
       <c r="B45" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C45">
         <v>0.5</v>
@@ -2131,13 +2155,13 @@
         <v>30</v>
       </c>
       <c r="G45" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="6"/>
       <c r="B46" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C46">
         <v>0.5</v>
@@ -2152,13 +2176,13 @@
         <v>30</v>
       </c>
       <c r="G46" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6"/>
       <c r="B47" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C47">
         <v>0.5</v>
@@ -2173,13 +2197,13 @@
         <v>30</v>
       </c>
       <c r="G47" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="6"/>
       <c r="B48" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C48">
         <v>0.5</v>
@@ -2194,13 +2218,13 @@
         <v>30</v>
       </c>
       <c r="G48" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="6"/>
       <c r="B49" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C49">
         <v>0.5</v>
@@ -2215,13 +2239,13 @@
         <v>30</v>
       </c>
       <c r="G49" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="6"/>
       <c r="B50" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C50">
         <v>0.5</v>
@@ -2236,13 +2260,13 @@
         <v>30</v>
       </c>
       <c r="G50" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="6"/>
       <c r="B51" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C51">
         <v>0.5</v>
@@ -2257,7 +2281,7 @@
         <v>30</v>
       </c>
       <c r="G51" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2278,7 +2302,7 @@
         <v>30</v>
       </c>
       <c r="G52" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2299,7 +2323,7 @@
         <v>30</v>
       </c>
       <c r="G53" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2320,13 +2344,13 @@
         <v>30</v>
       </c>
       <c r="G54" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="6"/>
       <c r="B55" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C55">
         <v>0.5</v>
@@ -2341,13 +2365,13 @@
         <v>30</v>
       </c>
       <c r="G55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="6"/>
       <c r="B56" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C56">
         <v>0.5</v>
@@ -2362,13 +2386,13 @@
         <v>30</v>
       </c>
       <c r="G56" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="6"/>
       <c r="B57" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -2383,13 +2407,13 @@
         <v>30</v>
       </c>
       <c r="G57" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="6"/>
       <c r="B58" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C58">
         <v>0.5</v>
@@ -2404,13 +2428,13 @@
         <v>30</v>
       </c>
       <c r="G58" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="6"/>
       <c r="B59" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C59">
         <v>0.5</v>
@@ -2425,13 +2449,13 @@
         <v>30</v>
       </c>
       <c r="G59" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="6"/>
       <c r="B60" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C60">
         <v>0.5</v>
@@ -2446,7 +2470,7 @@
         <v>30</v>
       </c>
       <c r="G60" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2464,10 +2488,10 @@
         <v>10</v>
       </c>
       <c r="F61" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G61" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2485,10 +2509,10 @@
         <v>10</v>
       </c>
       <c r="F62" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G62" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2506,37 +2530,40 @@
         <v>10</v>
       </c>
       <c r="F63" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G63" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="6"/>
       <c r="B64" t="s">
-        <v>125</v>
+        <v>210</v>
       </c>
       <c r="C64">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D64" t="s">
         <v>86</v>
       </c>
       <c r="E64" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+      <c r="G64" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="6"/>
       <c r="B65" t="s">
-        <v>126</v>
+        <v>212</v>
       </c>
       <c r="C65">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D65" t="s">
         <v>86</v>
@@ -2545,16 +2572,19 @@
         <v>9</v>
       </c>
       <c r="F65" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+      <c r="G65" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="6"/>
       <c r="B66" t="s">
-        <v>127</v>
+        <v>215</v>
       </c>
       <c r="C66">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D66" t="s">
         <v>86</v>
@@ -2565,14 +2595,17 @@
       <c r="F66" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G66" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="6"/>
       <c r="B67" t="s">
-        <v>128</v>
+        <v>217</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D67" t="s">
         <v>86</v>
@@ -2581,16 +2614,19 @@
         <v>9</v>
       </c>
       <c r="F67" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>218</v>
+      </c>
+      <c r="G67" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="6"/>
       <c r="B68" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C68">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D68" t="s">
         <v>86</v>
@@ -2599,13 +2635,13 @@
         <v>9</v>
       </c>
       <c r="F68" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="6"/>
       <c r="B69" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -2620,13 +2656,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="6"/>
       <c r="B70" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D70" t="s">
         <v>86</v>
@@ -2635,13 +2671,13 @@
         <v>9</v>
       </c>
       <c r="F70" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="6"/>
       <c r="B71" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -2653,13 +2689,13 @@
         <v>9</v>
       </c>
       <c r="F71" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="6"/>
       <c r="B72" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -2671,16 +2707,16 @@
         <v>9</v>
       </c>
       <c r="F72" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="6"/>
       <c r="B73" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C73">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D73" t="s">
         <v>86</v>
@@ -2689,16 +2725,16 @@
         <v>9</v>
       </c>
       <c r="F73" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="6"/>
       <c r="B74" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C74">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D74" t="s">
         <v>86</v>
@@ -2707,65 +2743,67 @@
         <v>9</v>
       </c>
       <c r="F74" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="6"/>
       <c r="B75" t="s">
+        <v>132</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75" t="s">
+        <v>86</v>
+      </c>
+      <c r="E75" t="s">
+        <v>9</v>
+      </c>
+      <c r="F75" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="6"/>
+      <c r="B76" t="s">
+        <v>133</v>
+      </c>
+      <c r="C76">
+        <v>5</v>
+      </c>
+      <c r="D76" t="s">
+        <v>86</v>
+      </c>
+      <c r="E76" t="s">
+        <v>9</v>
+      </c>
+      <c r="F76" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="6"/>
+      <c r="B77" t="s">
+        <v>134</v>
+      </c>
+      <c r="C77">
+        <v>2</v>
+      </c>
+      <c r="D77" t="s">
+        <v>86</v>
+      </c>
+      <c r="E77" t="s">
+        <v>9</v>
+      </c>
+      <c r="F77" t="s">
         <v>136</v>
       </c>
-      <c r="C75">
-        <v>3</v>
-      </c>
-      <c r="D75" t="s">
-        <v>86</v>
-      </c>
-      <c r="E75" t="s">
-        <v>9</v>
-      </c>
-      <c r="F75" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="3"/>
-      <c r="B76" t="s">
-        <v>207</v>
-      </c>
-      <c r="C76">
-        <v>1</v>
-      </c>
-      <c r="D76" t="s">
-        <v>86</v>
-      </c>
-      <c r="E76" t="s">
-        <v>9</v>
-      </c>
-      <c r="F76" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B77" t="s">
-        <v>139</v>
-      </c>
-      <c r="C77">
-        <v>2</v>
-      </c>
-      <c r="D77" t="s">
-        <v>86</v>
-      </c>
-      <c r="E77" t="s">
-        <v>9</v>
-      </c>
-      <c r="F77" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="78" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="6"/>
       <c r="B78" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C78">
         <v>3</v>
@@ -2777,15 +2815,16 @@
         <v>9</v>
       </c>
       <c r="F78" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="3"/>
       <c r="B79" t="s">
-        <v>141</v>
+        <v>206</v>
       </c>
       <c r="C79">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D79" t="s">
         <v>86</v>
@@ -2794,15 +2833,15 @@
         <v>9</v>
       </c>
       <c r="F79" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C80">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D80" t="s">
         <v>86</v>
@@ -2816,10 +2855,10 @@
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C81">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D81" t="s">
         <v>86</v>
@@ -2833,10 +2872,10 @@
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B82" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C82">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D82" t="s">
         <v>86</v>
@@ -2850,7 +2889,7 @@
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B83" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -2867,7 +2906,7 @@
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C84">
         <v>1</v>
@@ -2884,10 +2923,10 @@
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C85">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D85" t="s">
         <v>86</v>
@@ -2901,10 +2940,10 @@
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B86" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C86">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D86" t="s">
         <v>86</v>
@@ -2918,10 +2957,10 @@
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B87" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C87">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D87" t="s">
         <v>86</v>
@@ -2935,10 +2974,10 @@
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B88" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C88">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D88" t="s">
         <v>86</v>
@@ -2952,10 +2991,10 @@
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B89" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C89">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D89" t="s">
         <v>86</v>
@@ -2969,10 +3008,10 @@
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B90" t="s">
-        <v>62</v>
+        <v>149</v>
       </c>
       <c r="C90">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D90" t="s">
         <v>86</v>
@@ -2986,7 +3025,7 @@
     </row>
     <row r="91" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B91" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C91">
         <v>2</v>
@@ -3003,7 +3042,7 @@
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B92" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C92">
         <v>1</v>
@@ -3020,10 +3059,10 @@
     </row>
     <row r="93" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B93" t="s">
-        <v>154</v>
+        <v>62</v>
       </c>
       <c r="C93">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D93" t="s">
         <v>86</v>
@@ -3037,10 +3076,10 @@
     </row>
     <row r="94" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B94" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C94">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D94" t="s">
         <v>86</v>
@@ -3054,10 +3093,10 @@
     </row>
     <row r="95" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B95" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C95">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D95" t="s">
         <v>86</v>
@@ -3071,10 +3110,10 @@
     </row>
     <row r="96" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B96" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C96">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="D96" t="s">
         <v>86</v>
@@ -3088,10 +3127,10 @@
     </row>
     <row r="97" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B97" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C97">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D97" t="s">
         <v>86</v>
@@ -3105,10 +3144,10 @@
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B98" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C98">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D98" t="s">
         <v>86</v>
@@ -3122,67 +3161,58 @@
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B99" t="s">
-        <v>51</v>
+        <v>155</v>
       </c>
       <c r="C99">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D99" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="E99" t="s">
         <v>9</v>
       </c>
       <c r="F99" t="s">
         <v>29</v>
-      </c>
-      <c r="G99" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="100" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B100" t="s">
-        <v>14</v>
+        <v>157</v>
       </c>
       <c r="C100">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D100" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="E100" t="s">
         <v>9</v>
       </c>
       <c r="F100" t="s">
-        <v>31</v>
-      </c>
-      <c r="G100" s="1" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="101" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B101" t="s">
-        <v>13</v>
+        <v>158</v>
       </c>
       <c r="C101">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D101" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="E101" t="s">
         <v>9</v>
       </c>
       <c r="F101" t="s">
-        <v>31</v>
-      </c>
-      <c r="G101" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="102" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B102" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="C102">
         <v>3</v>
@@ -3194,18 +3224,18 @@
         <v>9</v>
       </c>
       <c r="F102" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
     </row>
     <row r="103" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B103" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C103">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D103" t="s">
         <v>2</v>
@@ -3217,15 +3247,15 @@
         <v>31</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="104" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B104" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C104">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D104" t="s">
         <v>2</v>
@@ -3237,15 +3267,15 @@
         <v>31</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B105" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C105">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D105" t="s">
         <v>2</v>
@@ -3257,15 +3287,15 @@
         <v>31</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B106" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C106">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D106" t="s">
         <v>2</v>
@@ -3277,15 +3307,15 @@
         <v>31</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B107" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C107">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D107" t="s">
         <v>2</v>
@@ -3297,75 +3327,75 @@
         <v>31</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="108" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B108" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C108">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D108" t="s">
         <v>2</v>
       </c>
       <c r="E108" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F108" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
     </row>
     <row r="109" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B109" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C109">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D109" t="s">
         <v>2</v>
       </c>
       <c r="E109" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F109" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="110" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B110" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="C110">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D110" t="s">
         <v>2</v>
       </c>
       <c r="E110" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F110" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
     </row>
     <row r="111" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B111" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C111">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D111" t="s">
         <v>2</v>
@@ -3377,15 +3407,15 @@
         <v>29</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="112" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B112" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="C112">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D112" t="s">
         <v>2</v>
@@ -3396,16 +3426,16 @@
       <c r="F112" t="s">
         <v>29</v>
       </c>
-      <c r="G112" t="s">
-        <v>85</v>
+      <c r="G112" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="113" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B113" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C113">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D113" t="s">
         <v>2</v>
@@ -3416,7 +3446,67 @@
       <c r="F113" t="s">
         <v>29</v>
       </c>
-      <c r="G113" t="s">
+      <c r="G113" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="114" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B114" t="s">
+        <v>48</v>
+      </c>
+      <c r="C114">
+        <v>3</v>
+      </c>
+      <c r="D114" t="s">
+        <v>2</v>
+      </c>
+      <c r="E114" t="s">
+        <v>12</v>
+      </c>
+      <c r="F114" t="s">
+        <v>29</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="115" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B115" t="s">
+        <v>67</v>
+      </c>
+      <c r="C115">
+        <v>1</v>
+      </c>
+      <c r="D115" t="s">
+        <v>2</v>
+      </c>
+      <c r="E115" t="s">
+        <v>12</v>
+      </c>
+      <c r="F115" t="s">
+        <v>29</v>
+      </c>
+      <c r="G115" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="116" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B116" t="s">
+        <v>55</v>
+      </c>
+      <c r="C116">
+        <v>1</v>
+      </c>
+      <c r="D116" t="s">
+        <v>2</v>
+      </c>
+      <c r="E116" t="s">
+        <v>12</v>
+      </c>
+      <c r="F116" t="s">
+        <v>29</v>
+      </c>
+      <c r="G116" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3424,39 +3514,39 @@
   <mergeCells count="4">
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A18"/>
-    <mergeCell ref="A35:A75"/>
+    <mergeCell ref="A35:A78"/>
     <mergeCell ref="A19:A34"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2 D4:D27 D105:D113 D116:D1048576 D29:D103">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2 D4:D27 D108:D116 D119:D1048576 D29:D106">
       <formula1>Types</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E105:E113 E116:E1048576 E2:E103">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E108:E116 E119:E1048576 E2:E106">
       <formula1>Statuses</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 F4:F27 F116:F1048576 F29:F113">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 F4:F27 F119:F1048576 F29:F116">
       <formula1>Themes</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G100" r:id="rId1"/>
-    <hyperlink ref="G102" r:id="rId2"/>
-    <hyperlink ref="G101" r:id="rId3"/>
-    <hyperlink ref="G103" r:id="rId4"/>
-    <hyperlink ref="G105" r:id="rId5"/>
-    <hyperlink ref="G104" r:id="rId6"/>
-    <hyperlink ref="G106" r:id="rId7"/>
-    <hyperlink ref="G107" r:id="rId8"/>
+    <hyperlink ref="G103" r:id="rId1"/>
+    <hyperlink ref="G105" r:id="rId2"/>
+    <hyperlink ref="G104" r:id="rId3"/>
+    <hyperlink ref="G106" r:id="rId4"/>
+    <hyperlink ref="G108" r:id="rId5"/>
+    <hyperlink ref="G107" r:id="rId6"/>
+    <hyperlink ref="G109" r:id="rId7"/>
+    <hyperlink ref="G110" r:id="rId8"/>
     <hyperlink ref="G2" r:id="rId9"/>
-    <hyperlink ref="G109" r:id="rId10"/>
-    <hyperlink ref="G108" r:id="rId11"/>
+    <hyperlink ref="G112" r:id="rId10"/>
+    <hyperlink ref="G111" r:id="rId11"/>
     <hyperlink ref="G3" r:id="rId12"/>
     <hyperlink ref="G4" r:id="rId13"/>
     <hyperlink ref="G5" r:id="rId14"/>
-    <hyperlink ref="G110" r:id="rId15"/>
+    <hyperlink ref="G113" r:id="rId15"/>
     <hyperlink ref="G6" r:id="rId16"/>
-    <hyperlink ref="G111" r:id="rId17"/>
-    <hyperlink ref="G99" r:id="rId18"/>
+    <hyperlink ref="G114" r:id="rId17"/>
+    <hyperlink ref="G102" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId19"/>
@@ -3465,10 +3555,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3523,7 +3613,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -3531,7 +3621,12 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>137</v>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the IAggregateRoot and IAggregateScope interfaces, in accordance with https://github.com/jonathanburrows/lavalav/issues/34
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -1190,7 +1190,7 @@
   <dimension ref="A1:G116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2548,7 +2548,7 @@
         <v>86</v>
       </c>
       <c r="E64" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F64" t="s">
         <v>137</v>
@@ -2569,7 +2569,7 @@
         <v>86</v>
       </c>
       <c r="E65" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F65" t="s">
         <v>137</v>

</xml_diff>

<commit_message>
adding headers service, in accordance with https://github.com/jonathanburrows/lavalav/issues/40
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="217">
   <si>
     <t>Name</t>
   </si>
@@ -744,12 +744,6 @@
   </si>
   <si>
     <t>Introduce the concept of aggregate scopes, so that DDD concepts can be applied.</t>
-  </si>
-  <si>
-    <t>Replace Xunit with Fluent Assertions, so that natural language can be used to describe unit tests.</t>
-  </si>
-  <si>
-    <t>Replace Xunit with FluentAssertions</t>
   </si>
   <si>
     <t>Investigate what SMWU would like, so that a proposal can be formed.</t>
@@ -1187,23 +1181,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G116"/>
+  <dimension ref="A1:G115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="195.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="195.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
@@ -1226,7 +1220,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>53</v>
       </c>
@@ -1249,7 +1243,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" t="s">
         <v>39</v>
@@ -1270,7 +1264,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>40</v>
@@ -1291,7 +1285,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
         <v>42</v>
@@ -1312,7 +1306,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>46</v>
@@ -1333,7 +1327,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>89</v>
       </c>
@@ -1356,7 +1350,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" t="s">
         <v>54</v>
@@ -1377,7 +1371,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" t="s">
         <v>56</v>
@@ -1398,7 +1392,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" t="s">
         <v>57</v>
@@ -1419,7 +1413,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" t="s">
         <v>58</v>
@@ -1440,7 +1434,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" t="s">
         <v>68</v>
@@ -1461,7 +1455,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" t="s">
         <v>59</v>
@@ -1482,7 +1476,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" t="s">
         <v>60</v>
@@ -1503,7 +1497,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" t="s">
         <v>61</v>
@@ -1524,7 +1518,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" t="s">
         <v>81</v>
@@ -1545,7 +1539,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" t="s">
         <v>63</v>
@@ -1566,7 +1560,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" t="s">
         <v>64</v>
@@ -1587,7 +1581,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>116</v>
       </c>
@@ -1610,7 +1604,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" t="s">
         <v>65</v>
@@ -1631,7 +1625,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" t="s">
         <v>66</v>
@@ -1652,7 +1646,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" t="s">
         <v>113</v>
@@ -1673,7 +1667,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" t="s">
         <v>114</v>
@@ -1694,7 +1688,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" t="s">
         <v>90</v>
@@ -1715,7 +1709,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" t="s">
         <v>92</v>
@@ -1736,7 +1730,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" t="s">
         <v>94</v>
@@ -1757,7 +1751,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" t="s">
         <v>96</v>
@@ -1778,7 +1772,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" t="s">
         <v>110</v>
@@ -1799,7 +1793,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" t="s">
         <v>98</v>
@@ -1820,7 +1814,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" t="s">
         <v>100</v>
@@ -1841,7 +1835,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" t="s">
         <v>102</v>
@@ -1862,7 +1856,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" t="s">
         <v>104</v>
@@ -1883,7 +1877,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" t="s">
         <v>106</v>
@@ -1904,7 +1898,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" t="s">
         <v>108</v>
@@ -1925,7 +1919,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>159</v>
       </c>
@@ -1948,7 +1942,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6"/>
       <c r="B36" t="s">
         <v>118</v>
@@ -1969,7 +1963,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" t="s">
         <v>161</v>
@@ -1990,7 +1984,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" t="s">
         <v>164</v>
@@ -2011,7 +2005,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6"/>
       <c r="B39" t="s">
         <v>166</v>
@@ -2032,7 +2026,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" t="s">
         <v>171</v>
@@ -2053,7 +2047,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" t="s">
         <v>169</v>
@@ -2074,7 +2068,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" t="s">
         <v>172</v>
@@ -2095,7 +2089,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" t="s">
         <v>174</v>
@@ -2116,7 +2110,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" t="s">
         <v>176</v>
@@ -2137,7 +2131,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" t="s">
         <v>183</v>
@@ -2158,7 +2152,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" t="s">
         <v>182</v>
@@ -2179,7 +2173,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" t="s">
         <v>181</v>
@@ -2200,7 +2194,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" t="s">
         <v>185</v>
@@ -2221,7 +2215,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" t="s">
         <v>186</v>
@@ -2242,7 +2236,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="B50" t="s">
         <v>186</v>
@@ -2263,7 +2257,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" t="s">
         <v>190</v>
@@ -2284,7 +2278,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" t="s">
         <v>119</v>
@@ -2305,7 +2299,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
       <c r="B53" t="s">
         <v>120</v>
@@ -2326,7 +2320,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
       <c r="B54" t="s">
         <v>121</v>
@@ -2347,7 +2341,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
       <c r="B55" t="s">
         <v>194</v>
@@ -2368,7 +2362,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="B56" t="s">
         <v>196</v>
@@ -2389,7 +2383,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" t="s">
         <v>198</v>
@@ -2410,7 +2404,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="B58" t="s">
         <v>200</v>
@@ -2431,7 +2425,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
       <c r="B59" t="s">
         <v>202</v>
@@ -2452,7 +2446,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
       <c r="B60" t="s">
         <v>204</v>
@@ -2473,7 +2467,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
       <c r="B61" t="s">
         <v>122</v>
@@ -2494,7 +2488,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
       <c r="B62" t="s">
         <v>123</v>
@@ -2515,7 +2509,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
       <c r="B63" t="s">
         <v>124</v>
@@ -2536,7 +2530,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="B64" t="s">
         <v>210</v>
@@ -2557,7 +2551,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
       <c r="B65" t="s">
         <v>212</v>
@@ -2569,7 +2563,7 @@
         <v>86</v>
       </c>
       <c r="E65" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F65" t="s">
         <v>137</v>
@@ -2578,13 +2572,13 @@
         <v>213</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
       <c r="B66" t="s">
         <v>215</v>
       </c>
       <c r="C66">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D66" t="s">
         <v>86</v>
@@ -2593,91 +2587,88 @@
         <v>9</v>
       </c>
       <c r="F66" t="s">
-        <v>30</v>
+        <v>216</v>
       </c>
       <c r="G66" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
       <c r="B67" t="s">
-        <v>217</v>
+        <v>125</v>
       </c>
       <c r="C67">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D67" t="s">
         <v>86</v>
       </c>
       <c r="E67" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F67" t="s">
-        <v>218</v>
-      </c>
-      <c r="G67" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6"/>
       <c r="B68" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D68" t="s">
         <v>86</v>
       </c>
       <c r="E68" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F68" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>
       <c r="B69" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D69" t="s">
         <v>86</v>
       </c>
       <c r="E69" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F69" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6"/>
       <c r="B70" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70" t="s">
         <v>86</v>
       </c>
       <c r="E70" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F70" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6"/>
       <c r="B71" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -2689,13 +2680,13 @@
         <v>9</v>
       </c>
       <c r="F71" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="6"/>
       <c r="B72" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -2704,16 +2695,16 @@
         <v>86</v>
       </c>
       <c r="E72" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F72" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6"/>
       <c r="B73" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -2722,16 +2713,16 @@
         <v>86</v>
       </c>
       <c r="E73" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
       <c r="B74" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -2743,16 +2734,16 @@
         <v>9</v>
       </c>
       <c r="F74" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
       <c r="B75" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C75">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D75" t="s">
         <v>86</v>
@@ -2764,13 +2755,13 @@
         <v>137</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
       <c r="B76" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C76">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D76" t="s">
         <v>86</v>
@@ -2779,16 +2770,16 @@
         <v>9</v>
       </c>
       <c r="F76" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
       <c r="B77" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C77">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D77" t="s">
         <v>86</v>
@@ -2797,52 +2788,51 @@
         <v>9</v>
       </c>
       <c r="F77" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="6"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="3"/>
       <c r="B78" t="s">
-        <v>135</v>
+        <v>206</v>
       </c>
       <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="D78" t="s">
+        <v>86</v>
+      </c>
+      <c r="E78" t="s">
+        <v>9</v>
+      </c>
+      <c r="F78" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>138</v>
+      </c>
+      <c r="C79">
+        <v>2</v>
+      </c>
+      <c r="D79" t="s">
+        <v>86</v>
+      </c>
+      <c r="E79" t="s">
+        <v>9</v>
+      </c>
+      <c r="F79" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>139</v>
+      </c>
+      <c r="C80">
         <v>3</v>
       </c>
-      <c r="D78" t="s">
-        <v>86</v>
-      </c>
-      <c r="E78" t="s">
-        <v>9</v>
-      </c>
-      <c r="F78" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="3"/>
-      <c r="B79" t="s">
-        <v>206</v>
-      </c>
-      <c r="C79">
-        <v>1</v>
-      </c>
-      <c r="D79" t="s">
-        <v>86</v>
-      </c>
-      <c r="E79" t="s">
-        <v>9</v>
-      </c>
-      <c r="F79" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B80" t="s">
-        <v>138</v>
-      </c>
-      <c r="C80">
-        <v>2</v>
-      </c>
       <c r="D80" t="s">
         <v>86</v>
       </c>
@@ -2853,64 +2843,64 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C81">
+        <v>2</v>
+      </c>
+      <c r="D81" t="s">
+        <v>86</v>
+      </c>
+      <c r="E81" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>142</v>
+      </c>
+      <c r="C82">
+        <v>1</v>
+      </c>
+      <c r="D82" t="s">
+        <v>86</v>
+      </c>
+      <c r="E82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F82" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>141</v>
+      </c>
+      <c r="C83">
+        <v>1</v>
+      </c>
+      <c r="D83" t="s">
+        <v>86</v>
+      </c>
+      <c r="E83" t="s">
+        <v>9</v>
+      </c>
+      <c r="F83" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>145</v>
+      </c>
+      <c r="C84">
         <v>3</v>
       </c>
-      <c r="D81" t="s">
-        <v>86</v>
-      </c>
-      <c r="E81" t="s">
-        <v>9</v>
-      </c>
-      <c r="F81" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B82" t="s">
-        <v>140</v>
-      </c>
-      <c r="C82">
-        <v>2</v>
-      </c>
-      <c r="D82" t="s">
-        <v>86</v>
-      </c>
-      <c r="E82" t="s">
-        <v>9</v>
-      </c>
-      <c r="F82" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B83" t="s">
-        <v>142</v>
-      </c>
-      <c r="C83">
-        <v>1</v>
-      </c>
-      <c r="D83" t="s">
-        <v>86</v>
-      </c>
-      <c r="E83" t="s">
-        <v>9</v>
-      </c>
-      <c r="F83" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B84" t="s">
-        <v>141</v>
-      </c>
-      <c r="C84">
-        <v>1</v>
-      </c>
       <c r="D84" t="s">
         <v>86</v>
       </c>
@@ -2921,217 +2911,217 @@
         <v>29</v>
       </c>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85" t="s">
+        <v>86</v>
+      </c>
+      <c r="E85" t="s">
+        <v>9</v>
+      </c>
+      <c r="F85" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>147</v>
+      </c>
+      <c r="C86">
+        <v>1</v>
+      </c>
+      <c r="D86" t="s">
+        <v>86</v>
+      </c>
+      <c r="E86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F86" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>143</v>
+      </c>
+      <c r="C87">
+        <v>1</v>
+      </c>
+      <c r="D87" t="s">
+        <v>86</v>
+      </c>
+      <c r="E87" t="s">
+        <v>9</v>
+      </c>
+      <c r="F87" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>144</v>
+      </c>
+      <c r="C88">
+        <v>2</v>
+      </c>
+      <c r="D88" t="s">
+        <v>86</v>
+      </c>
+      <c r="E88" t="s">
+        <v>9</v>
+      </c>
+      <c r="F88" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>149</v>
+      </c>
+      <c r="C89">
+        <v>2</v>
+      </c>
+      <c r="D89" t="s">
+        <v>86</v>
+      </c>
+      <c r="E89" t="s">
+        <v>9</v>
+      </c>
+      <c r="F89" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>150</v>
+      </c>
+      <c r="C90">
+        <v>2</v>
+      </c>
+      <c r="D90" t="s">
+        <v>86</v>
+      </c>
+      <c r="E90" t="s">
+        <v>9</v>
+      </c>
+      <c r="F90" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>148</v>
+      </c>
+      <c r="C91">
+        <v>1</v>
+      </c>
+      <c r="D91" t="s">
+        <v>86</v>
+      </c>
+      <c r="E91" t="s">
+        <v>9</v>
+      </c>
+      <c r="F91" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>62</v>
+      </c>
+      <c r="C92">
+        <v>1</v>
+      </c>
+      <c r="D92" t="s">
+        <v>86</v>
+      </c>
+      <c r="E92" t="s">
+        <v>9</v>
+      </c>
+      <c r="F92" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>151</v>
+      </c>
+      <c r="C93">
+        <v>2</v>
+      </c>
+      <c r="D93" t="s">
+        <v>86</v>
+      </c>
+      <c r="E93" t="s">
+        <v>9</v>
+      </c>
+      <c r="F93" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>152</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+      <c r="D94" t="s">
+        <v>86</v>
+      </c>
+      <c r="E94" t="s">
+        <v>9</v>
+      </c>
+      <c r="F94" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>153</v>
+      </c>
+      <c r="C95">
+        <v>0.5</v>
+      </c>
+      <c r="D95" t="s">
+        <v>86</v>
+      </c>
+      <c r="E95" t="s">
+        <v>9</v>
+      </c>
+      <c r="F95" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>156</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+      <c r="D96" t="s">
+        <v>86</v>
+      </c>
+      <c r="E96" t="s">
+        <v>9</v>
+      </c>
+      <c r="F96" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>154</v>
+      </c>
+      <c r="C97">
         <v>3</v>
       </c>
-      <c r="D85" t="s">
-        <v>86</v>
-      </c>
-      <c r="E85" t="s">
-        <v>9</v>
-      </c>
-      <c r="F85" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B86" t="s">
-        <v>146</v>
-      </c>
-      <c r="C86">
-        <v>1</v>
-      </c>
-      <c r="D86" t="s">
-        <v>86</v>
-      </c>
-      <c r="E86" t="s">
-        <v>9</v>
-      </c>
-      <c r="F86" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B87" t="s">
-        <v>147</v>
-      </c>
-      <c r="C87">
-        <v>1</v>
-      </c>
-      <c r="D87" t="s">
-        <v>86</v>
-      </c>
-      <c r="E87" t="s">
-        <v>9</v>
-      </c>
-      <c r="F87" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B88" t="s">
-        <v>143</v>
-      </c>
-      <c r="C88">
-        <v>1</v>
-      </c>
-      <c r="D88" t="s">
-        <v>86</v>
-      </c>
-      <c r="E88" t="s">
-        <v>9</v>
-      </c>
-      <c r="F88" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B89" t="s">
-        <v>144</v>
-      </c>
-      <c r="C89">
-        <v>2</v>
-      </c>
-      <c r="D89" t="s">
-        <v>86</v>
-      </c>
-      <c r="E89" t="s">
-        <v>9</v>
-      </c>
-      <c r="F89" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B90" t="s">
-        <v>149</v>
-      </c>
-      <c r="C90">
-        <v>2</v>
-      </c>
-      <c r="D90" t="s">
-        <v>86</v>
-      </c>
-      <c r="E90" t="s">
-        <v>9</v>
-      </c>
-      <c r="F90" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B91" t="s">
-        <v>150</v>
-      </c>
-      <c r="C91">
-        <v>2</v>
-      </c>
-      <c r="D91" t="s">
-        <v>86</v>
-      </c>
-      <c r="E91" t="s">
-        <v>9</v>
-      </c>
-      <c r="F91" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B92" t="s">
-        <v>148</v>
-      </c>
-      <c r="C92">
-        <v>1</v>
-      </c>
-      <c r="D92" t="s">
-        <v>86</v>
-      </c>
-      <c r="E92" t="s">
-        <v>9</v>
-      </c>
-      <c r="F92" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B93" t="s">
-        <v>62</v>
-      </c>
-      <c r="C93">
-        <v>1</v>
-      </c>
-      <c r="D93" t="s">
-        <v>86</v>
-      </c>
-      <c r="E93" t="s">
-        <v>9</v>
-      </c>
-      <c r="F93" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B94" t="s">
-        <v>151</v>
-      </c>
-      <c r="C94">
-        <v>2</v>
-      </c>
-      <c r="D94" t="s">
-        <v>86</v>
-      </c>
-      <c r="E94" t="s">
-        <v>9</v>
-      </c>
-      <c r="F94" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B95" t="s">
-        <v>152</v>
-      </c>
-      <c r="C95">
-        <v>1</v>
-      </c>
-      <c r="D95" t="s">
-        <v>86</v>
-      </c>
-      <c r="E95" t="s">
-        <v>9</v>
-      </c>
-      <c r="F95" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B96" t="s">
-        <v>153</v>
-      </c>
-      <c r="C96">
-        <v>0.5</v>
-      </c>
-      <c r="D96" t="s">
-        <v>86</v>
-      </c>
-      <c r="E96" t="s">
-        <v>9</v>
-      </c>
-      <c r="F96" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B97" t="s">
-        <v>156</v>
-      </c>
-      <c r="C97">
-        <v>1</v>
-      </c>
       <c r="D97" t="s">
         <v>86</v>
       </c>
@@ -3142,66 +3132,66 @@
         <v>29</v>
       </c>
     </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C98">
+        <v>2</v>
+      </c>
+      <c r="D98" t="s">
+        <v>86</v>
+      </c>
+      <c r="E98" t="s">
+        <v>9</v>
+      </c>
+      <c r="F98" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>157</v>
+      </c>
+      <c r="C99">
+        <v>2</v>
+      </c>
+      <c r="D99" t="s">
+        <v>86</v>
+      </c>
+      <c r="E99" t="s">
+        <v>9</v>
+      </c>
+      <c r="F99" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>158</v>
+      </c>
+      <c r="C100">
+        <v>5</v>
+      </c>
+      <c r="D100" t="s">
+        <v>86</v>
+      </c>
+      <c r="E100" t="s">
+        <v>9</v>
+      </c>
+      <c r="F100" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>51</v>
+      </c>
+      <c r="C101">
         <v>3</v>
       </c>
-      <c r="D98" t="s">
-        <v>86</v>
-      </c>
-      <c r="E98" t="s">
-        <v>9</v>
-      </c>
-      <c r="F98" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B99" t="s">
-        <v>155</v>
-      </c>
-      <c r="C99">
-        <v>2</v>
-      </c>
-      <c r="D99" t="s">
-        <v>86</v>
-      </c>
-      <c r="E99" t="s">
-        <v>9</v>
-      </c>
-      <c r="F99" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B100" t="s">
-        <v>157</v>
-      </c>
-      <c r="C100">
-        <v>2</v>
-      </c>
-      <c r="D100" t="s">
-        <v>86</v>
-      </c>
-      <c r="E100" t="s">
-        <v>9</v>
-      </c>
-      <c r="F100" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B101" t="s">
-        <v>158</v>
-      </c>
-      <c r="C101">
-        <v>5</v>
-      </c>
       <c r="D101" t="s">
-        <v>86</v>
+        <v>2</v>
       </c>
       <c r="E101" t="s">
         <v>9</v>
@@ -3209,13 +3199,16 @@
       <c r="F101" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="G101" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="C102">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D102" t="s">
         <v>2</v>
@@ -3224,15 +3217,15 @@
         <v>9</v>
       </c>
       <c r="F102" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C103">
         <v>1</v>
@@ -3247,15 +3240,15 @@
         <v>31</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C104">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D104" t="s">
         <v>2</v>
@@ -3267,15 +3260,15 @@
         <v>31</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C105">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D105" t="s">
         <v>2</v>
@@ -3287,15 +3280,15 @@
         <v>31</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C106">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D106" t="s">
         <v>2</v>
@@ -3307,15 +3300,15 @@
         <v>31</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C107">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D107" t="s">
         <v>2</v>
@@ -3327,15 +3320,15 @@
         <v>31</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C108">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D108" t="s">
         <v>2</v>
@@ -3347,12 +3340,12 @@
         <v>31</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C109">
         <v>1</v>
@@ -3367,35 +3360,35 @@
         <v>31</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C110">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D110" t="s">
         <v>2</v>
       </c>
       <c r="E110" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F110" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C111">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D111" t="s">
         <v>2</v>
@@ -3407,15 +3400,15 @@
         <v>29</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C112">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D112" t="s">
         <v>2</v>
@@ -3427,15 +3420,15 @@
         <v>29</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C113">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D113" t="s">
         <v>2</v>
@@ -3447,15 +3440,15 @@
         <v>29</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="C114">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D114" t="s">
         <v>2</v>
@@ -3466,13 +3459,13 @@
       <c r="F114" t="s">
         <v>29</v>
       </c>
-      <c r="G114" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="G114" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C115">
         <v>1</v>
@@ -3487,26 +3480,6 @@
         <v>29</v>
       </c>
       <c r="G115" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B116" t="s">
-        <v>55</v>
-      </c>
-      <c r="C116">
-        <v>1</v>
-      </c>
-      <c r="D116" t="s">
-        <v>2</v>
-      </c>
-      <c r="E116" t="s">
-        <v>12</v>
-      </c>
-      <c r="F116" t="s">
-        <v>29</v>
-      </c>
-      <c r="G116" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3514,39 +3487,39 @@
   <mergeCells count="4">
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A18"/>
-    <mergeCell ref="A35:A78"/>
+    <mergeCell ref="A35:A77"/>
     <mergeCell ref="A19:A34"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2 D4:D27 D108:D116 D119:D1048576 D29:D106">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2 D4:D27 D107:D115 D118:D1048576 D29:D105">
       <formula1>Types</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E108:E116 E119:E1048576 E2:E106">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E107:E115 E118:E1048576 E2:E105">
       <formula1>Statuses</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 F4:F27 F119:F1048576 F29:F116">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 F4:F27 F118:F1048576 F29:F115">
       <formula1>Themes</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G103" r:id="rId1"/>
-    <hyperlink ref="G105" r:id="rId2"/>
-    <hyperlink ref="G104" r:id="rId3"/>
-    <hyperlink ref="G106" r:id="rId4"/>
-    <hyperlink ref="G108" r:id="rId5"/>
-    <hyperlink ref="G107" r:id="rId6"/>
-    <hyperlink ref="G109" r:id="rId7"/>
-    <hyperlink ref="G110" r:id="rId8"/>
+    <hyperlink ref="G102" r:id="rId1"/>
+    <hyperlink ref="G104" r:id="rId2"/>
+    <hyperlink ref="G103" r:id="rId3"/>
+    <hyperlink ref="G105" r:id="rId4"/>
+    <hyperlink ref="G107" r:id="rId5"/>
+    <hyperlink ref="G106" r:id="rId6"/>
+    <hyperlink ref="G108" r:id="rId7"/>
+    <hyperlink ref="G109" r:id="rId8"/>
     <hyperlink ref="G2" r:id="rId9"/>
-    <hyperlink ref="G112" r:id="rId10"/>
-    <hyperlink ref="G111" r:id="rId11"/>
+    <hyperlink ref="G111" r:id="rId10"/>
+    <hyperlink ref="G110" r:id="rId11"/>
     <hyperlink ref="G3" r:id="rId12"/>
     <hyperlink ref="G4" r:id="rId13"/>
     <hyperlink ref="G5" r:id="rId14"/>
-    <hyperlink ref="G113" r:id="rId15"/>
+    <hyperlink ref="G112" r:id="rId15"/>
     <hyperlink ref="G6" r:id="rId16"/>
-    <hyperlink ref="G114" r:id="rId17"/>
-    <hyperlink ref="G102" r:id="rId18"/>
+    <hyperlink ref="G113" r:id="rId17"/>
+    <hyperlink ref="G101" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId19"/>
@@ -3561,13 +3534,13 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -3578,7 +3551,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3589,7 +3562,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -3600,7 +3573,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -3608,7 +3581,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -3616,7 +3589,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -3624,9 +3597,9 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added front end options, in accordance with https://github.com/jonathanburrows/lavalav/issues/41
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -1183,7 +1183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
       <selection activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
@@ -2677,7 +2677,7 @@
         <v>86</v>
       </c>
       <c r="E71" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" t="s">
         <v>30</v>
@@ -2713,7 +2713,7 @@
         <v>86</v>
       </c>
       <c r="E73" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F73" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
adding layout component, in accordance with https://github.com/jonathanburrows/lavalav/issues/48
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="219">
   <si>
     <t>Name</t>
   </si>
@@ -753,6 +753,12 @@
   </si>
   <si>
     <t>SMWU</t>
+  </si>
+  <si>
+    <t>Roboto Font</t>
+  </si>
+  <si>
+    <t>Add regular and icon Roboto fonts, so that it can adhere to material guidelines.</t>
   </si>
 </sst>
 </file>
@@ -849,10 +855,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1181,23 +1190,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G115"/>
+  <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="F73" sqref="F73"/>
+    <sheetView tabSelected="1" topLeftCell="B63" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="195.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="195.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
@@ -1220,8 +1229,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
         <v>53</v>
       </c>
       <c r="B2" t="s">
@@ -1243,8 +1252,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="5"/>
       <c r="B3" t="s">
         <v>39</v>
       </c>
@@ -1264,8 +1273,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="5"/>
       <c r="B4" t="s">
         <v>40</v>
       </c>
@@ -1285,8 +1294,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5"/>
       <c r="B5" t="s">
         <v>42</v>
       </c>
@@ -1306,8 +1315,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="5"/>
       <c r="B6" t="s">
         <v>46</v>
       </c>
@@ -1327,8 +1336,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
         <v>89</v>
       </c>
       <c r="B7" t="s">
@@ -1350,8 +1359,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6"/>
       <c r="B8" t="s">
         <v>54</v>
       </c>
@@ -1371,8 +1380,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="6"/>
       <c r="B9" t="s">
         <v>56</v>
       </c>
@@ -1392,8 +1401,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="6"/>
       <c r="B10" t="s">
         <v>57</v>
       </c>
@@ -1413,8 +1422,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="6"/>
       <c r="B11" t="s">
         <v>58</v>
       </c>
@@ -1434,8 +1443,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="6"/>
       <c r="B12" t="s">
         <v>68</v>
       </c>
@@ -1455,8 +1464,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="6"/>
       <c r="B13" t="s">
         <v>59</v>
       </c>
@@ -1476,8 +1485,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="6"/>
       <c r="B14" t="s">
         <v>60</v>
       </c>
@@ -1497,8 +1506,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="6"/>
       <c r="B15" t="s">
         <v>61</v>
       </c>
@@ -1518,8 +1527,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="6"/>
       <c r="B16" t="s">
         <v>81</v>
       </c>
@@ -1539,8 +1548,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="6"/>
       <c r="B17" t="s">
         <v>63</v>
       </c>
@@ -1560,8 +1569,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="6"/>
       <c r="B18" t="s">
         <v>64</v>
       </c>
@@ -1581,8 +1590,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="8" t="s">
         <v>116</v>
       </c>
       <c r="B19" t="s">
@@ -1604,8 +1613,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="8"/>
       <c r="B20" t="s">
         <v>65</v>
       </c>
@@ -1625,8 +1634,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="8"/>
       <c r="B21" t="s">
         <v>66</v>
       </c>
@@ -1646,8 +1655,8 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="8"/>
       <c r="B22" t="s">
         <v>113</v>
       </c>
@@ -1667,8 +1676,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="8"/>
       <c r="B23" t="s">
         <v>114</v>
       </c>
@@ -1688,8 +1697,8 @@
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="8"/>
       <c r="B24" t="s">
         <v>90</v>
       </c>
@@ -1709,8 +1718,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="8"/>
       <c r="B25" t="s">
         <v>92</v>
       </c>
@@ -1730,8 +1739,8 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
+    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="8"/>
       <c r="B26" t="s">
         <v>94</v>
       </c>
@@ -1751,8 +1760,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="8"/>
       <c r="B27" t="s">
         <v>96</v>
       </c>
@@ -1772,8 +1781,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="8"/>
       <c r="B28" t="s">
         <v>110</v>
       </c>
@@ -1793,8 +1802,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="8"/>
       <c r="B29" t="s">
         <v>98</v>
       </c>
@@ -1814,8 +1823,8 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="8"/>
       <c r="B30" t="s">
         <v>100</v>
       </c>
@@ -1835,8 +1844,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="8"/>
       <c r="B31" t="s">
         <v>102</v>
       </c>
@@ -1856,8 +1865,8 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
+    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="8"/>
       <c r="B32" t="s">
         <v>104</v>
       </c>
@@ -1877,8 +1886,8 @@
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="8"/>
       <c r="B33" t="s">
         <v>106</v>
       </c>
@@ -1898,8 +1907,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="8"/>
       <c r="B34" t="s">
         <v>108</v>
       </c>
@@ -1919,8 +1928,8 @@
         <v>109</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="6" t="s">
+    <row r="35" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="7" t="s">
         <v>159</v>
       </c>
       <c r="B35" t="s">
@@ -1942,8 +1951,8 @@
         <v>160</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="6"/>
+    <row r="36" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="7"/>
       <c r="B36" t="s">
         <v>118</v>
       </c>
@@ -1963,8 +1972,8 @@
         <v>163</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
+    <row r="37" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="7"/>
       <c r="B37" t="s">
         <v>161</v>
       </c>
@@ -1984,8 +1993,8 @@
         <v>162</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
+    <row r="38" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="7"/>
       <c r="B38" t="s">
         <v>164</v>
       </c>
@@ -2005,8 +2014,8 @@
         <v>165</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="6"/>
+    <row r="39" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="7"/>
       <c r="B39" t="s">
         <v>166</v>
       </c>
@@ -2026,8 +2035,8 @@
         <v>167</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
+    <row r="40" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="7"/>
       <c r="B40" t="s">
         <v>171</v>
       </c>
@@ -2047,8 +2056,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
+    <row r="41" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="7"/>
       <c r="B41" t="s">
         <v>169</v>
       </c>
@@ -2068,8 +2077,8 @@
         <v>170</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
+    <row r="42" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="7"/>
       <c r="B42" t="s">
         <v>172</v>
       </c>
@@ -2089,8 +2098,8 @@
         <v>173</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
+    <row r="43" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="7"/>
       <c r="B43" t="s">
         <v>174</v>
       </c>
@@ -2110,8 +2119,8 @@
         <v>175</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
+    <row r="44" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="7"/>
       <c r="B44" t="s">
         <v>176</v>
       </c>
@@ -2131,8 +2140,8 @@
         <v>177</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
+    <row r="45" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="7"/>
       <c r="B45" t="s">
         <v>183</v>
       </c>
@@ -2152,8 +2161,8 @@
         <v>179</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
+    <row r="46" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="7"/>
       <c r="B46" t="s">
         <v>182</v>
       </c>
@@ -2173,8 +2182,8 @@
         <v>178</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
+    <row r="47" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="7"/>
       <c r="B47" t="s">
         <v>181</v>
       </c>
@@ -2194,8 +2203,8 @@
         <v>180</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
+    <row r="48" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="7"/>
       <c r="B48" t="s">
         <v>185</v>
       </c>
@@ -2215,8 +2224,8 @@
         <v>184</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
+    <row r="49" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="7"/>
       <c r="B49" t="s">
         <v>186</v>
       </c>
@@ -2236,8 +2245,8 @@
         <v>187</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
+    <row r="50" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="7"/>
       <c r="B50" t="s">
         <v>186</v>
       </c>
@@ -2257,8 +2266,8 @@
         <v>188</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
+    <row r="51" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="7"/>
       <c r="B51" t="s">
         <v>190</v>
       </c>
@@ -2278,8 +2287,8 @@
         <v>191</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="6"/>
+    <row r="52" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="7"/>
       <c r="B52" t="s">
         <v>119</v>
       </c>
@@ -2299,8 +2308,8 @@
         <v>189</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="6"/>
+    <row r="53" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="7"/>
       <c r="B53" t="s">
         <v>120</v>
       </c>
@@ -2320,8 +2329,8 @@
         <v>192</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
+    <row r="54" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="7"/>
       <c r="B54" t="s">
         <v>121</v>
       </c>
@@ -2341,8 +2350,8 @@
         <v>193</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="6"/>
+    <row r="55" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="7"/>
       <c r="B55" t="s">
         <v>194</v>
       </c>
@@ -2362,8 +2371,8 @@
         <v>195</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="6"/>
+    <row r="56" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="7"/>
       <c r="B56" t="s">
         <v>196</v>
       </c>
@@ -2383,8 +2392,8 @@
         <v>197</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="6"/>
+    <row r="57" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="7"/>
       <c r="B57" t="s">
         <v>198</v>
       </c>
@@ -2404,8 +2413,8 @@
         <v>199</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="6"/>
+    <row r="58" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="7"/>
       <c r="B58" t="s">
         <v>200</v>
       </c>
@@ -2425,8 +2434,8 @@
         <v>201</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="6"/>
+    <row r="59" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="7"/>
       <c r="B59" t="s">
         <v>202</v>
       </c>
@@ -2446,8 +2455,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="6"/>
+    <row r="60" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="7"/>
       <c r="B60" t="s">
         <v>204</v>
       </c>
@@ -2467,8 +2476,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="6"/>
+    <row r="61" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="7"/>
       <c r="B61" t="s">
         <v>122</v>
       </c>
@@ -2488,8 +2497,8 @@
         <v>208</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="6"/>
+    <row r="62" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="7"/>
       <c r="B62" t="s">
         <v>123</v>
       </c>
@@ -2509,8 +2518,8 @@
         <v>207</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="6"/>
+    <row r="63" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="7"/>
       <c r="B63" t="s">
         <v>124</v>
       </c>
@@ -2530,8 +2539,8 @@
         <v>209</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="6"/>
+    <row r="64" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="7"/>
       <c r="B64" t="s">
         <v>210</v>
       </c>
@@ -2551,8 +2560,8 @@
         <v>211</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="6"/>
+    <row r="65" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="7"/>
       <c r="B65" t="s">
         <v>212</v>
       </c>
@@ -2572,8 +2581,8 @@
         <v>213</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="6"/>
+    <row r="66" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="7"/>
       <c r="B66" t="s">
         <v>215</v>
       </c>
@@ -2584,7 +2593,7 @@
         <v>86</v>
       </c>
       <c r="E66" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F66" t="s">
         <v>216</v>
@@ -2593,8 +2602,8 @@
         <v>214</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="6"/>
+    <row r="67" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="7"/>
       <c r="B67" t="s">
         <v>125</v>
       </c>
@@ -2611,8 +2620,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="6"/>
+    <row r="68" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="7"/>
       <c r="B68" t="s">
         <v>126</v>
       </c>
@@ -2629,8 +2638,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="6"/>
+    <row r="69" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="7"/>
       <c r="B69" t="s">
         <v>127</v>
       </c>
@@ -2647,8 +2656,8 @@
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="6"/>
+    <row r="70" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="7"/>
       <c r="B70" t="s">
         <v>128</v>
       </c>
@@ -2665,8 +2674,8 @@
         <v>136</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="6"/>
+    <row r="71" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="7"/>
       <c r="B71" t="s">
         <v>129</v>
       </c>
@@ -2677,14 +2686,14 @@
         <v>86</v>
       </c>
       <c r="E71" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F71" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="6"/>
+    <row r="72" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="7"/>
       <c r="B72" t="s">
         <v>130</v>
       </c>
@@ -2701,8 +2710,8 @@
         <v>137</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="6"/>
+    <row r="73" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="7"/>
       <c r="B73" t="s">
         <v>131</v>
       </c>
@@ -2719,8 +2728,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="6"/>
+    <row r="74" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="7"/>
       <c r="B74" t="s">
         <v>132</v>
       </c>
@@ -2731,14 +2740,14 @@
         <v>86</v>
       </c>
       <c r="E74" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F74" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="6"/>
+    <row r="75" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="7"/>
       <c r="B75" t="s">
         <v>133</v>
       </c>
@@ -2755,8 +2764,8 @@
         <v>137</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="6"/>
+    <row r="76" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="7"/>
       <c r="B76" t="s">
         <v>134</v>
       </c>
@@ -2773,8 +2782,8 @@
         <v>136</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="6"/>
+    <row r="77" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="7"/>
       <c r="B77" t="s">
         <v>135</v>
       </c>
@@ -2785,53 +2794,57 @@
         <v>86</v>
       </c>
       <c r="E77" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="3"/>
+    <row r="78" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="4"/>
       <c r="B78" t="s">
+        <v>217</v>
+      </c>
+      <c r="C78">
+        <v>0.5</v>
+      </c>
+      <c r="D78" t="s">
+        <v>86</v>
+      </c>
+      <c r="E78" t="s">
+        <v>10</v>
+      </c>
+      <c r="F78" t="s">
+        <v>136</v>
+      </c>
+      <c r="G78" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="3"/>
+      <c r="B79" t="s">
         <v>206</v>
       </c>
-      <c r="C78">
-        <v>1</v>
-      </c>
-      <c r="D78" t="s">
-        <v>86</v>
-      </c>
-      <c r="E78" t="s">
-        <v>9</v>
-      </c>
-      <c r="F78" t="s">
+      <c r="C79">
+        <v>1</v>
+      </c>
+      <c r="D79" t="s">
+        <v>86</v>
+      </c>
+      <c r="E79" t="s">
+        <v>10</v>
+      </c>
+      <c r="F79" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B80" t="s">
         <v>138</v>
       </c>
-      <c r="C79">
-        <v>2</v>
-      </c>
-      <c r="D79" t="s">
-        <v>86</v>
-      </c>
-      <c r="E79" t="s">
-        <v>9</v>
-      </c>
-      <c r="F79" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>139</v>
-      </c>
       <c r="C80">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D80" t="s">
         <v>86</v>
@@ -2843,12 +2856,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C81">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D81" t="s">
         <v>86</v>
@@ -2860,12 +2873,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B82" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C82">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D82" t="s">
         <v>86</v>
@@ -2877,9 +2890,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B83" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -2894,12 +2907,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C84">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2911,12 +2924,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C85">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D85" t="s">
         <v>86</v>
@@ -2928,9 +2941,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B86" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C86">
         <v>1</v>
@@ -2945,9 +2958,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B87" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C87">
         <v>1</v>
@@ -2962,12 +2975,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B88" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C88">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D88" t="s">
         <v>86</v>
@@ -2979,9 +2992,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B89" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C89">
         <v>2</v>
@@ -2996,9 +3009,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B90" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C90">
         <v>2</v>
@@ -3013,12 +3026,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B91" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C91">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D91" t="s">
         <v>86</v>
@@ -3030,9 +3043,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B92" t="s">
-        <v>62</v>
+        <v>148</v>
       </c>
       <c r="C92">
         <v>1</v>
@@ -3047,12 +3060,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B93" t="s">
-        <v>151</v>
+        <v>62</v>
       </c>
       <c r="C93">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D93" t="s">
         <v>86</v>
@@ -3064,12 +3077,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B94" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C94">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D94" t="s">
         <v>86</v>
@@ -3081,12 +3094,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B95" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C95">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D95" t="s">
         <v>86</v>
@@ -3098,12 +3111,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B96" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C96">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D96" t="s">
         <v>86</v>
@@ -3115,12 +3128,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B97" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C97">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D97" t="s">
         <v>86</v>
@@ -3132,12 +3145,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B98" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C98">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D98" t="s">
         <v>86</v>
@@ -3149,9 +3162,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B99" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C99">
         <v>2</v>
@@ -3166,12 +3179,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B100" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C100">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D100" t="s">
         <v>86</v>
@@ -3183,15 +3196,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B101" t="s">
-        <v>51</v>
+        <v>158</v>
       </c>
       <c r="C101">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D101" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="E101" t="s">
         <v>9</v>
@@ -3199,16 +3212,13 @@
       <c r="F101" t="s">
         <v>29</v>
       </c>
-      <c r="G101" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B102" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="C102">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D102" t="s">
         <v>2</v>
@@ -3217,15 +3227,15 @@
         <v>9</v>
       </c>
       <c r="F102" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B103" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C103">
         <v>1</v>
@@ -3240,15 +3250,15 @@
         <v>31</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B104" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C104">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D104" t="s">
         <v>2</v>
@@ -3260,15 +3270,15 @@
         <v>31</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B105" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C105">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D105" t="s">
         <v>2</v>
@@ -3280,15 +3290,15 @@
         <v>31</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="106" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B106" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C106">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D106" t="s">
         <v>2</v>
@@ -3300,15 +3310,15 @@
         <v>31</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="107" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B107" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C107">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D107" t="s">
         <v>2</v>
@@ -3320,15 +3330,15 @@
         <v>31</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B108" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C108">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D108" t="s">
         <v>2</v>
@@ -3340,12 +3350,12 @@
         <v>31</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B109" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C109">
         <v>1</v>
@@ -3360,35 +3370,35 @@
         <v>31</v>
       </c>
       <c r="G109" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B110" t="s">
+        <v>25</v>
+      </c>
+      <c r="C110">
+        <v>1</v>
+      </c>
+      <c r="D110" t="s">
+        <v>2</v>
+      </c>
+      <c r="E110" t="s">
+        <v>9</v>
+      </c>
+      <c r="F110" t="s">
+        <v>31</v>
+      </c>
+      <c r="G110" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
+    <row r="111" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B111" t="s">
         <v>37</v>
       </c>
-      <c r="C110">
+      <c r="C111">
         <v>8</v>
-      </c>
-      <c r="D110" t="s">
-        <v>2</v>
-      </c>
-      <c r="E110" t="s">
-        <v>12</v>
-      </c>
-      <c r="F110" t="s">
-        <v>29</v>
-      </c>
-      <c r="G110" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B111" t="s">
-        <v>34</v>
-      </c>
-      <c r="C111">
-        <v>3</v>
       </c>
       <c r="D111" t="s">
         <v>2</v>
@@ -3400,15 +3410,15 @@
         <v>29</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="112" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B112" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C112">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D112" t="s">
         <v>2</v>
@@ -3420,15 +3430,15 @@
         <v>29</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="113" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B113" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C113">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D113" t="s">
         <v>2</v>
@@ -3440,15 +3450,15 @@
         <v>29</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="114" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B114" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="C114">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D114" t="s">
         <v>2</v>
@@ -3459,13 +3469,13 @@
       <c r="F114" t="s">
         <v>29</v>
       </c>
-      <c r="G114" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G114" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="115" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B115" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="C115">
         <v>1</v>
@@ -3480,6 +3490,26 @@
         <v>29</v>
       </c>
       <c r="G115" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="116" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B116" t="s">
+        <v>55</v>
+      </c>
+      <c r="C116">
+        <v>1</v>
+      </c>
+      <c r="D116" t="s">
+        <v>2</v>
+      </c>
+      <c r="E116" t="s">
+        <v>12</v>
+      </c>
+      <c r="F116" t="s">
+        <v>29</v>
+      </c>
+      <c r="G116" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3491,35 +3521,35 @@
     <mergeCell ref="A19:A34"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2 D4:D27 D107:D115 D118:D1048576 D29:D105">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2 D4:D27 D108:D116 D119:D1048576 D29:D106">
       <formula1>Types</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E107:E115 E118:E1048576 E2:E105">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E108:E116 E119:E1048576 E2:E106">
       <formula1>Statuses</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 F4:F27 F118:F1048576 F29:F115">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 F4:F27 F119:F1048576 F29:F116">
       <formula1>Themes</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G102" r:id="rId1"/>
-    <hyperlink ref="G104" r:id="rId2"/>
-    <hyperlink ref="G103" r:id="rId3"/>
-    <hyperlink ref="G105" r:id="rId4"/>
-    <hyperlink ref="G107" r:id="rId5"/>
-    <hyperlink ref="G106" r:id="rId6"/>
-    <hyperlink ref="G108" r:id="rId7"/>
-    <hyperlink ref="G109" r:id="rId8"/>
+    <hyperlink ref="G103" r:id="rId1"/>
+    <hyperlink ref="G105" r:id="rId2"/>
+    <hyperlink ref="G104" r:id="rId3"/>
+    <hyperlink ref="G106" r:id="rId4"/>
+    <hyperlink ref="G108" r:id="rId5"/>
+    <hyperlink ref="G107" r:id="rId6"/>
+    <hyperlink ref="G109" r:id="rId7"/>
+    <hyperlink ref="G110" r:id="rId8"/>
     <hyperlink ref="G2" r:id="rId9"/>
-    <hyperlink ref="G111" r:id="rId10"/>
-    <hyperlink ref="G110" r:id="rId11"/>
+    <hyperlink ref="G112" r:id="rId10"/>
+    <hyperlink ref="G111" r:id="rId11"/>
     <hyperlink ref="G3" r:id="rId12"/>
     <hyperlink ref="G4" r:id="rId13"/>
     <hyperlink ref="G5" r:id="rId14"/>
-    <hyperlink ref="G112" r:id="rId15"/>
+    <hyperlink ref="G113" r:id="rId15"/>
     <hyperlink ref="G6" r:id="rId16"/>
-    <hyperlink ref="G113" r:id="rId17"/>
-    <hyperlink ref="G101" r:id="rId18"/>
+    <hyperlink ref="G114" r:id="rId17"/>
+    <hyperlink ref="G102" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId19"/>
@@ -3534,13 +3564,13 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -3551,7 +3581,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3562,7 +3592,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -3573,7 +3603,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -3581,7 +3611,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -3589,7 +3619,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -3597,7 +3627,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
         <v>216</v>
       </c>

</xml_diff>

<commit_message>
adding validation, in accordance with https://github.com/jonathanburrows/lavalav/issues/50
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="220">
   <si>
     <t>Name</t>
   </si>
@@ -759,6 +759,9 @@
   </si>
   <si>
     <t>Add regular and icon Roboto fonts, so that it can adhere to material guidelines.</t>
+  </si>
+  <si>
+    <t>Create a set of validation helpers, so that validation does not need to be done manually in each form.</t>
   </si>
 </sst>
 </file>
@@ -1192,21 +1195,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B63" workbookViewId="0">
-      <selection activeCell="E77" sqref="E77"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="195.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="195.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
@@ -1229,7 +1232,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>53</v>
       </c>
@@ -1252,7 +1255,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" t="s">
         <v>39</v>
@@ -1273,7 +1276,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" t="s">
         <v>40</v>
@@ -1294,7 +1297,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" t="s">
         <v>42</v>
@@ -1315,7 +1318,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" t="s">
         <v>46</v>
@@ -1336,7 +1339,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>89</v>
       </c>
@@ -1359,7 +1362,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" t="s">
         <v>54</v>
@@ -1380,7 +1383,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" t="s">
         <v>56</v>
@@ -1401,7 +1404,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" t="s">
         <v>57</v>
@@ -1422,7 +1425,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" t="s">
         <v>58</v>
@@ -1443,7 +1446,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" t="s">
         <v>68</v>
@@ -1464,7 +1467,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" t="s">
         <v>59</v>
@@ -1485,7 +1488,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" t="s">
         <v>60</v>
@@ -1506,7 +1509,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" t="s">
         <v>61</v>
@@ -1527,7 +1530,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" t="s">
         <v>81</v>
@@ -1548,7 +1551,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" t="s">
         <v>63</v>
@@ -1569,7 +1572,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" t="s">
         <v>64</v>
@@ -1590,7 +1593,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>116</v>
       </c>
@@ -1613,7 +1616,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" t="s">
         <v>65</v>
@@ -1634,7 +1637,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" t="s">
         <v>66</v>
@@ -1655,7 +1658,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" t="s">
         <v>113</v>
@@ -1676,7 +1679,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" t="s">
         <v>114</v>
@@ -1697,7 +1700,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" t="s">
         <v>90</v>
@@ -1718,7 +1721,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" t="s">
         <v>92</v>
@@ -1739,7 +1742,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" t="s">
         <v>94</v>
@@ -1760,7 +1763,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" t="s">
         <v>96</v>
@@ -1781,7 +1784,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" t="s">
         <v>110</v>
@@ -1802,7 +1805,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" t="s">
         <v>98</v>
@@ -1823,7 +1826,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" t="s">
         <v>100</v>
@@ -1844,7 +1847,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" t="s">
         <v>102</v>
@@ -1865,7 +1868,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" t="s">
         <v>104</v>
@@ -1886,7 +1889,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" t="s">
         <v>106</v>
@@ -1907,7 +1910,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" t="s">
         <v>108</v>
@@ -1928,7 +1931,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>159</v>
       </c>
@@ -1951,7 +1954,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7"/>
       <c r="B36" t="s">
         <v>118</v>
@@ -1972,7 +1975,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" t="s">
         <v>161</v>
@@ -1993,7 +1996,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" t="s">
         <v>164</v>
@@ -2014,7 +2017,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7"/>
       <c r="B39" t="s">
         <v>166</v>
@@ -2035,7 +2038,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" t="s">
         <v>171</v>
@@ -2056,7 +2059,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" t="s">
         <v>169</v>
@@ -2077,7 +2080,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" t="s">
         <v>172</v>
@@ -2098,7 +2101,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" t="s">
         <v>174</v>
@@ -2119,7 +2122,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" t="s">
         <v>176</v>
@@ -2140,7 +2143,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" t="s">
         <v>183</v>
@@ -2161,7 +2164,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" t="s">
         <v>182</v>
@@ -2182,7 +2185,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" t="s">
         <v>181</v>
@@ -2203,7 +2206,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" t="s">
         <v>185</v>
@@ -2224,7 +2227,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" t="s">
         <v>186</v>
@@ -2245,7 +2248,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" t="s">
         <v>186</v>
@@ -2266,7 +2269,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" t="s">
         <v>190</v>
@@ -2287,7 +2290,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" t="s">
         <v>119</v>
@@ -2308,7 +2311,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" t="s">
         <v>120</v>
@@ -2329,7 +2332,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" t="s">
         <v>121</v>
@@ -2350,7 +2353,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" t="s">
         <v>194</v>
@@ -2371,7 +2374,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" t="s">
         <v>196</v>
@@ -2392,7 +2395,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" t="s">
         <v>198</v>
@@ -2413,7 +2416,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
       <c r="B58" t="s">
         <v>200</v>
@@ -2434,7 +2437,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
       <c r="B59" t="s">
         <v>202</v>
@@ -2455,7 +2458,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
       <c r="B60" t="s">
         <v>204</v>
@@ -2476,7 +2479,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="B61" t="s">
         <v>122</v>
@@ -2497,7 +2500,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
       <c r="B62" t="s">
         <v>123</v>
@@ -2518,7 +2521,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7"/>
       <c r="B63" t="s">
         <v>124</v>
@@ -2539,7 +2542,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7"/>
       <c r="B64" t="s">
         <v>210</v>
@@ -2560,7 +2563,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7"/>
       <c r="B65" t="s">
         <v>212</v>
@@ -2581,7 +2584,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
       <c r="B66" t="s">
         <v>215</v>
@@ -2602,7 +2605,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7"/>
       <c r="B67" t="s">
         <v>125</v>
@@ -2620,7 +2623,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
       <c r="B68" t="s">
         <v>126</v>
@@ -2638,7 +2641,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="7"/>
       <c r="B69" t="s">
         <v>127</v>
@@ -2656,7 +2659,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
       <c r="B70" t="s">
         <v>128</v>
@@ -2674,7 +2677,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
       <c r="B71" t="s">
         <v>129</v>
@@ -2692,7 +2695,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7"/>
       <c r="B72" t="s">
         <v>130</v>
@@ -2710,7 +2713,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
       <c r="B73" t="s">
         <v>131</v>
@@ -2728,7 +2731,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="7"/>
       <c r="B74" t="s">
         <v>132</v>
@@ -2746,7 +2749,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="7"/>
       <c r="B75" t="s">
         <v>133</v>
@@ -2758,13 +2761,16 @@
         <v>86</v>
       </c>
       <c r="E75" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F75" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G75" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="7"/>
       <c r="B76" t="s">
         <v>134</v>
@@ -2782,7 +2788,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="7"/>
       <c r="B77" t="s">
         <v>135</v>
@@ -2794,13 +2800,13 @@
         <v>86</v>
       </c>
       <c r="E77" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F77" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" t="s">
         <v>217</v>
@@ -2821,7 +2827,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" t="s">
         <v>206</v>
@@ -2839,7 +2845,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>138</v>
       </c>
@@ -2856,7 +2862,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>139</v>
       </c>
@@ -2873,7 +2879,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>140</v>
       </c>
@@ -2890,7 +2896,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>142</v>
       </c>
@@ -2907,7 +2913,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>141</v>
       </c>
@@ -2924,7 +2930,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>145</v>
       </c>
@@ -2941,7 +2947,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>146</v>
       </c>
@@ -2958,7 +2964,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>147</v>
       </c>
@@ -2975,7 +2981,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>143</v>
       </c>
@@ -2992,7 +2998,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>144</v>
       </c>
@@ -3009,7 +3015,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>149</v>
       </c>
@@ -3026,7 +3032,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>150</v>
       </c>
@@ -3043,7 +3049,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>148</v>
       </c>
@@ -3060,7 +3066,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>62</v>
       </c>
@@ -3077,7 +3083,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>151</v>
       </c>
@@ -3094,7 +3100,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>152</v>
       </c>
@@ -3111,7 +3117,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>153</v>
       </c>
@@ -3128,7 +3134,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>156</v>
       </c>
@@ -3145,7 +3151,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>154</v>
       </c>
@@ -3162,7 +3168,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>155</v>
       </c>
@@ -3179,7 +3185,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>157</v>
       </c>
@@ -3196,7 +3202,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>158</v>
       </c>
@@ -3213,7 +3219,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>51</v>
       </c>
@@ -3233,7 +3239,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>14</v>
       </c>
@@ -3253,7 +3259,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>13</v>
       </c>
@@ -3273,7 +3279,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>1</v>
       </c>
@@ -3293,7 +3299,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>18</v>
       </c>
@@ -3313,7 +3319,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>22</v>
       </c>
@@ -3333,7 +3339,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>21</v>
       </c>
@@ -3353,7 +3359,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>23</v>
       </c>
@@ -3373,7 +3379,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>25</v>
       </c>
@@ -3393,7 +3399,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>37</v>
       </c>
@@ -3413,7 +3419,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>34</v>
       </c>
@@ -3433,7 +3439,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>45</v>
       </c>
@@ -3453,7 +3459,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>48</v>
       </c>
@@ -3473,7 +3479,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>67</v>
       </c>
@@ -3493,7 +3499,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>55</v>
       </c>
@@ -3564,13 +3570,13 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -3581,7 +3587,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3592,7 +3598,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -3603,7 +3609,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -3611,7 +3617,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -3619,7 +3625,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -3627,7 +3633,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>216</v>
       </c>

</xml_diff>

<commit_message>
adding oidc project, in accordance with https://github.com/jonathanburrows/lavalav/issues/77
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="249">
   <si>
     <t>Name</t>
   </si>
@@ -1282,8 +1282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B104" sqref="B104"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2925,7 +2925,7 @@
         <v>86</v>
       </c>
       <c r="E79" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F79" t="s">
         <v>29</v>
@@ -2945,7 +2945,7 @@
         <v>86</v>
       </c>
       <c r="E80" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F80" t="s">
         <v>29</v>
@@ -2965,7 +2965,7 @@
         <v>86</v>
       </c>
       <c r="E81" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F81" t="s">
         <v>29</v>
@@ -2985,7 +2985,7 @@
         <v>86</v>
       </c>
       <c r="E82" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F82" t="s">
         <v>29</v>
@@ -3005,7 +3005,7 @@
         <v>86</v>
       </c>
       <c r="E83" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F83" t="s">
         <v>29</v>

</xml_diff>